<commit_message>
building component labor input and cost tables extended to 1900 to cover renovation history generation
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_BuildingComponent_Input_Labor.xlsx
+++ b/projects/test_building/input/Scenario_BuildingComponent_Input_Labor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="50" yWindow="4310" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="45" yWindow="4305" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="157">
   <si>
     <t>id_region</t>
   </si>
@@ -160,6 +160,336 @@
   </si>
   <si>
     <t>person-hour/m2</t>
+  </si>
+  <si>
+    <t>1900</t>
+  </si>
+  <si>
+    <t>1901</t>
+  </si>
+  <si>
+    <t>1902</t>
+  </si>
+  <si>
+    <t>1903</t>
+  </si>
+  <si>
+    <t>1904</t>
+  </si>
+  <si>
+    <t>1905</t>
+  </si>
+  <si>
+    <t>1906</t>
+  </si>
+  <si>
+    <t>1907</t>
+  </si>
+  <si>
+    <t>1908</t>
+  </si>
+  <si>
+    <t>1909</t>
+  </si>
+  <si>
+    <t>1910</t>
+  </si>
+  <si>
+    <t>1911</t>
+  </si>
+  <si>
+    <t>1912</t>
+  </si>
+  <si>
+    <t>1913</t>
+  </si>
+  <si>
+    <t>1914</t>
+  </si>
+  <si>
+    <t>1915</t>
+  </si>
+  <si>
+    <t>1916</t>
+  </si>
+  <si>
+    <t>1917</t>
+  </si>
+  <si>
+    <t>1918</t>
+  </si>
+  <si>
+    <t>1919</t>
+  </si>
+  <si>
+    <t>1920</t>
+  </si>
+  <si>
+    <t>1921</t>
+  </si>
+  <si>
+    <t>1922</t>
+  </si>
+  <si>
+    <t>1923</t>
+  </si>
+  <si>
+    <t>1924</t>
+  </si>
+  <si>
+    <t>1925</t>
+  </si>
+  <si>
+    <t>1926</t>
+  </si>
+  <si>
+    <t>1927</t>
+  </si>
+  <si>
+    <t>1928</t>
+  </si>
+  <si>
+    <t>1929</t>
+  </si>
+  <si>
+    <t>1930</t>
+  </si>
+  <si>
+    <t>1931</t>
+  </si>
+  <si>
+    <t>1932</t>
+  </si>
+  <si>
+    <t>1933</t>
+  </si>
+  <si>
+    <t>1934</t>
+  </si>
+  <si>
+    <t>1935</t>
+  </si>
+  <si>
+    <t>1936</t>
+  </si>
+  <si>
+    <t>1937</t>
+  </si>
+  <si>
+    <t>1938</t>
+  </si>
+  <si>
+    <t>1939</t>
+  </si>
+  <si>
+    <t>1940</t>
+  </si>
+  <si>
+    <t>1941</t>
+  </si>
+  <si>
+    <t>1942</t>
+  </si>
+  <si>
+    <t>1943</t>
+  </si>
+  <si>
+    <t>1944</t>
+  </si>
+  <si>
+    <t>1945</t>
+  </si>
+  <si>
+    <t>1946</t>
+  </si>
+  <si>
+    <t>1947</t>
+  </si>
+  <si>
+    <t>1948</t>
+  </si>
+  <si>
+    <t>1949</t>
+  </si>
+  <si>
+    <t>1950</t>
+  </si>
+  <si>
+    <t>1951</t>
+  </si>
+  <si>
+    <t>1952</t>
+  </si>
+  <si>
+    <t>1953</t>
+  </si>
+  <si>
+    <t>1954</t>
+  </si>
+  <si>
+    <t>1955</t>
+  </si>
+  <si>
+    <t>1956</t>
+  </si>
+  <si>
+    <t>1957</t>
+  </si>
+  <si>
+    <t>1958</t>
+  </si>
+  <si>
+    <t>1959</t>
+  </si>
+  <si>
+    <t>1960</t>
+  </si>
+  <si>
+    <t>1961</t>
+  </si>
+  <si>
+    <t>1962</t>
+  </si>
+  <si>
+    <t>1963</t>
+  </si>
+  <si>
+    <t>1964</t>
+  </si>
+  <si>
+    <t>1965</t>
+  </si>
+  <si>
+    <t>1966</t>
+  </si>
+  <si>
+    <t>1967</t>
+  </si>
+  <si>
+    <t>1968</t>
+  </si>
+  <si>
+    <t>1969</t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>1971</t>
+  </si>
+  <si>
+    <t>1972</t>
+  </si>
+  <si>
+    <t>1973</t>
+  </si>
+  <si>
+    <t>1974</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>1976</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>1979</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>1983</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
   </si>
 </sst>
 </file>
@@ -225,14 +555,124 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AT11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:AT11"/>
-  <tableColumns count="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:EZ11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:EZ11"/>
+  <tableColumns count="156">
     <tableColumn id="1" name="id_region"/>
     <tableColumn id="3" name="id_building_component"/>
     <tableColumn id="4" name="id_building_component_option"/>
     <tableColumn id="5" name="id_building_action"/>
     <tableColumn id="6" name="unit"/>
+    <tableColumn id="88" name="1900"/>
+    <tableColumn id="89" name="1901"/>
+    <tableColumn id="90" name="1902"/>
+    <tableColumn id="91" name="1903"/>
+    <tableColumn id="92" name="1904"/>
+    <tableColumn id="93" name="1905"/>
+    <tableColumn id="94" name="1906"/>
+    <tableColumn id="95" name="1907"/>
+    <tableColumn id="96" name="1908"/>
+    <tableColumn id="97" name="1909"/>
+    <tableColumn id="98" name="1910"/>
+    <tableColumn id="99" name="1911"/>
+    <tableColumn id="100" name="1912"/>
+    <tableColumn id="101" name="1913"/>
+    <tableColumn id="102" name="1914"/>
+    <tableColumn id="103" name="1915"/>
+    <tableColumn id="104" name="1916"/>
+    <tableColumn id="105" name="1917"/>
+    <tableColumn id="106" name="1918"/>
+    <tableColumn id="107" name="1919"/>
+    <tableColumn id="108" name="1920"/>
+    <tableColumn id="109" name="1921"/>
+    <tableColumn id="110" name="1922"/>
+    <tableColumn id="111" name="1923"/>
+    <tableColumn id="112" name="1924"/>
+    <tableColumn id="113" name="1925"/>
+    <tableColumn id="114" name="1926"/>
+    <tableColumn id="115" name="1927"/>
+    <tableColumn id="116" name="1928"/>
+    <tableColumn id="117" name="1929"/>
+    <tableColumn id="118" name="1930"/>
+    <tableColumn id="119" name="1931"/>
+    <tableColumn id="120" name="1932"/>
+    <tableColumn id="121" name="1933"/>
+    <tableColumn id="122" name="1934"/>
+    <tableColumn id="123" name="1935"/>
+    <tableColumn id="124" name="1936"/>
+    <tableColumn id="125" name="1937"/>
+    <tableColumn id="126" name="1938"/>
+    <tableColumn id="127" name="1939"/>
+    <tableColumn id="128" name="1940"/>
+    <tableColumn id="129" name="1941"/>
+    <tableColumn id="130" name="1942"/>
+    <tableColumn id="131" name="1943"/>
+    <tableColumn id="132" name="1944"/>
+    <tableColumn id="133" name="1945"/>
+    <tableColumn id="134" name="1946"/>
+    <tableColumn id="135" name="1947"/>
+    <tableColumn id="136" name="1948"/>
+    <tableColumn id="137" name="1949"/>
+    <tableColumn id="138" name="1950"/>
+    <tableColumn id="139" name="1951"/>
+    <tableColumn id="140" name="1952"/>
+    <tableColumn id="141" name="1953"/>
+    <tableColumn id="142" name="1954"/>
+    <tableColumn id="143" name="1955"/>
+    <tableColumn id="144" name="1956"/>
+    <tableColumn id="145" name="1957"/>
+    <tableColumn id="146" name="1958"/>
+    <tableColumn id="147" name="1959"/>
+    <tableColumn id="148" name="1960"/>
+    <tableColumn id="149" name="1961"/>
+    <tableColumn id="150" name="1962"/>
+    <tableColumn id="151" name="1963"/>
+    <tableColumn id="152" name="1964"/>
+    <tableColumn id="153" name="1965"/>
+    <tableColumn id="154" name="1966"/>
+    <tableColumn id="155" name="1967"/>
+    <tableColumn id="156" name="1968"/>
+    <tableColumn id="157" name="1969"/>
+    <tableColumn id="158" name="1970"/>
+    <tableColumn id="159" name="1971"/>
+    <tableColumn id="160" name="1972"/>
+    <tableColumn id="161" name="1973"/>
+    <tableColumn id="162" name="1974"/>
+    <tableColumn id="163" name="1975"/>
+    <tableColumn id="164" name="1976"/>
+    <tableColumn id="165" name="1977"/>
+    <tableColumn id="166" name="1978"/>
+    <tableColumn id="167" name="1979"/>
+    <tableColumn id="168" name="1980"/>
+    <tableColumn id="169" name="1981"/>
+    <tableColumn id="2" name="1982"/>
+    <tableColumn id="48" name="1983"/>
+    <tableColumn id="49" name="1984"/>
+    <tableColumn id="50" name="1985"/>
+    <tableColumn id="51" name="1986"/>
+    <tableColumn id="52" name="1987"/>
+    <tableColumn id="53" name="1988"/>
+    <tableColumn id="54" name="1989"/>
+    <tableColumn id="55" name="1990"/>
+    <tableColumn id="56" name="1991"/>
+    <tableColumn id="57" name="1992"/>
+    <tableColumn id="58" name="1993"/>
+    <tableColumn id="59" name="1994"/>
+    <tableColumn id="60" name="1995"/>
+    <tableColumn id="61" name="1996"/>
+    <tableColumn id="62" name="1997"/>
+    <tableColumn id="63" name="1998"/>
+    <tableColumn id="64" name="1999"/>
+    <tableColumn id="65" name="2000"/>
+    <tableColumn id="66" name="2001"/>
+    <tableColumn id="67" name="2002"/>
+    <tableColumn id="68" name="2003"/>
+    <tableColumn id="69" name="2004"/>
+    <tableColumn id="70" name="2005"/>
+    <tableColumn id="71" name="2006"/>
+    <tableColumn id="72" name="2007"/>
+    <tableColumn id="73" name="2008"/>
+    <tableColumn id="74" name="2009"/>
     <tableColumn id="7" name="2010"/>
     <tableColumn id="8" name="2011"/>
     <tableColumn id="9" name="2012"/>
@@ -542,22 +982,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT11"/>
+  <dimension ref="A1:EZ11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="156" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,130 +1015,460 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>114</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>115</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>123</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>125</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>126</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>128</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>129</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>130</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>131</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>133</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>134</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>135</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>136</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>138</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>139</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>140</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>141</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>142</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>143</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>144</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>145</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>146</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>147</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>148</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>150</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>154</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>155</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DL1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="DM1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="DN1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="DO1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="DP1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="DQ1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="DR1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="DS1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="DT1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="DU1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="DV1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="DW1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="DX1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="DY1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="DZ1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="EA1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="EB1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="EC1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="ED1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="EE1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="EF1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="EG1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="EH1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="EI1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="EJ1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="EK1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="EL1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="EM1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="EN1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="EO1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="EP1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="EQ1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="ER1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="ES1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="ET1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="EU1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="EV1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="EW1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="EX1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="EY1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="EZ1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -836,8 +1607,338 @@
       <c r="AT2">
         <v>1</v>
       </c>
+      <c r="AU2">
+        <v>1</v>
+      </c>
+      <c r="AV2">
+        <v>1</v>
+      </c>
+      <c r="AW2">
+        <v>1</v>
+      </c>
+      <c r="AX2">
+        <v>1</v>
+      </c>
+      <c r="AY2">
+        <v>1</v>
+      </c>
+      <c r="AZ2">
+        <v>1</v>
+      </c>
+      <c r="BA2">
+        <v>1</v>
+      </c>
+      <c r="BB2">
+        <v>1</v>
+      </c>
+      <c r="BC2">
+        <v>1</v>
+      </c>
+      <c r="BD2">
+        <v>1</v>
+      </c>
+      <c r="BE2">
+        <v>1</v>
+      </c>
+      <c r="BF2">
+        <v>1</v>
+      </c>
+      <c r="BG2">
+        <v>1</v>
+      </c>
+      <c r="BH2">
+        <v>1</v>
+      </c>
+      <c r="BI2">
+        <v>1</v>
+      </c>
+      <c r="BJ2">
+        <v>1</v>
+      </c>
+      <c r="BK2">
+        <v>1</v>
+      </c>
+      <c r="BL2">
+        <v>1</v>
+      </c>
+      <c r="BM2">
+        <v>1</v>
+      </c>
+      <c r="BN2">
+        <v>1</v>
+      </c>
+      <c r="BO2">
+        <v>1</v>
+      </c>
+      <c r="BP2">
+        <v>1</v>
+      </c>
+      <c r="BQ2">
+        <v>1</v>
+      </c>
+      <c r="BR2">
+        <v>1</v>
+      </c>
+      <c r="BS2">
+        <v>1</v>
+      </c>
+      <c r="BT2">
+        <v>1</v>
+      </c>
+      <c r="BU2">
+        <v>1</v>
+      </c>
+      <c r="BV2">
+        <v>1</v>
+      </c>
+      <c r="BW2">
+        <v>1</v>
+      </c>
+      <c r="BX2">
+        <v>1</v>
+      </c>
+      <c r="BY2">
+        <v>1</v>
+      </c>
+      <c r="BZ2">
+        <v>1</v>
+      </c>
+      <c r="CA2">
+        <v>1</v>
+      </c>
+      <c r="CB2">
+        <v>1</v>
+      </c>
+      <c r="CC2">
+        <v>1</v>
+      </c>
+      <c r="CD2">
+        <v>1</v>
+      </c>
+      <c r="CE2">
+        <v>1</v>
+      </c>
+      <c r="CF2">
+        <v>1</v>
+      </c>
+      <c r="CG2">
+        <v>1</v>
+      </c>
+      <c r="CH2">
+        <v>1</v>
+      </c>
+      <c r="CI2">
+        <v>1</v>
+      </c>
+      <c r="CJ2">
+        <v>1</v>
+      </c>
+      <c r="CK2">
+        <v>1</v>
+      </c>
+      <c r="CL2">
+        <v>1</v>
+      </c>
+      <c r="CM2">
+        <v>1</v>
+      </c>
+      <c r="CN2">
+        <v>1</v>
+      </c>
+      <c r="CO2">
+        <v>1</v>
+      </c>
+      <c r="CP2">
+        <v>1</v>
+      </c>
+      <c r="CQ2">
+        <v>1</v>
+      </c>
+      <c r="CR2">
+        <v>1</v>
+      </c>
+      <c r="CS2">
+        <v>1</v>
+      </c>
+      <c r="CT2">
+        <v>1</v>
+      </c>
+      <c r="CU2">
+        <v>1</v>
+      </c>
+      <c r="CV2">
+        <v>1</v>
+      </c>
+      <c r="CW2">
+        <v>1</v>
+      </c>
+      <c r="CX2">
+        <v>1</v>
+      </c>
+      <c r="CY2">
+        <v>1</v>
+      </c>
+      <c r="CZ2">
+        <v>1</v>
+      </c>
+      <c r="DA2">
+        <v>1</v>
+      </c>
+      <c r="DB2">
+        <v>1</v>
+      </c>
+      <c r="DC2">
+        <v>1</v>
+      </c>
+      <c r="DD2">
+        <v>1</v>
+      </c>
+      <c r="DE2">
+        <v>1</v>
+      </c>
+      <c r="DF2">
+        <v>1</v>
+      </c>
+      <c r="DG2">
+        <v>1</v>
+      </c>
+      <c r="DH2">
+        <v>1</v>
+      </c>
+      <c r="DI2">
+        <v>1</v>
+      </c>
+      <c r="DJ2">
+        <v>1</v>
+      </c>
+      <c r="DK2">
+        <v>1</v>
+      </c>
+      <c r="DL2">
+        <v>1</v>
+      </c>
+      <c r="DM2">
+        <v>1</v>
+      </c>
+      <c r="DN2">
+        <v>1</v>
+      </c>
+      <c r="DO2">
+        <v>1</v>
+      </c>
+      <c r="DP2">
+        <v>1</v>
+      </c>
+      <c r="DQ2">
+        <v>1</v>
+      </c>
+      <c r="DR2">
+        <v>1</v>
+      </c>
+      <c r="DS2">
+        <v>1</v>
+      </c>
+      <c r="DT2">
+        <v>1</v>
+      </c>
+      <c r="DU2">
+        <v>1</v>
+      </c>
+      <c r="DV2">
+        <v>1</v>
+      </c>
+      <c r="DW2">
+        <v>1</v>
+      </c>
+      <c r="DX2">
+        <v>1</v>
+      </c>
+      <c r="DY2">
+        <v>1</v>
+      </c>
+      <c r="DZ2">
+        <v>1</v>
+      </c>
+      <c r="EA2">
+        <v>1</v>
+      </c>
+      <c r="EB2">
+        <v>1</v>
+      </c>
+      <c r="EC2">
+        <v>1</v>
+      </c>
+      <c r="ED2">
+        <v>1</v>
+      </c>
+      <c r="EE2">
+        <v>1</v>
+      </c>
+      <c r="EF2">
+        <v>1</v>
+      </c>
+      <c r="EG2">
+        <v>1</v>
+      </c>
+      <c r="EH2">
+        <v>1</v>
+      </c>
+      <c r="EI2">
+        <v>1</v>
+      </c>
+      <c r="EJ2">
+        <v>1</v>
+      </c>
+      <c r="EK2">
+        <v>1</v>
+      </c>
+      <c r="EL2">
+        <v>1</v>
+      </c>
+      <c r="EM2">
+        <v>1</v>
+      </c>
+      <c r="EN2">
+        <v>1</v>
+      </c>
+      <c r="EO2">
+        <v>1</v>
+      </c>
+      <c r="EP2">
+        <v>1</v>
+      </c>
+      <c r="EQ2">
+        <v>1</v>
+      </c>
+      <c r="ER2">
+        <v>1</v>
+      </c>
+      <c r="ES2">
+        <v>1</v>
+      </c>
+      <c r="ET2">
+        <v>1</v>
+      </c>
+      <c r="EU2">
+        <v>1</v>
+      </c>
+      <c r="EV2">
+        <v>1</v>
+      </c>
+      <c r="EW2">
+        <v>1</v>
+      </c>
+      <c r="EX2">
+        <v>1</v>
+      </c>
+      <c r="EY2">
+        <v>1</v>
+      </c>
+      <c r="EZ2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -976,8 +2077,338 @@
       <c r="AT3">
         <v>1.34</v>
       </c>
+      <c r="AU3">
+        <v>1.34</v>
+      </c>
+      <c r="AV3">
+        <v>1.34</v>
+      </c>
+      <c r="AW3">
+        <v>1.34</v>
+      </c>
+      <c r="AX3">
+        <v>1.34</v>
+      </c>
+      <c r="AY3">
+        <v>1.34</v>
+      </c>
+      <c r="AZ3">
+        <v>1.34</v>
+      </c>
+      <c r="BA3">
+        <v>1.34</v>
+      </c>
+      <c r="BB3">
+        <v>1.34</v>
+      </c>
+      <c r="BC3">
+        <v>1.34</v>
+      </c>
+      <c r="BD3">
+        <v>1.34</v>
+      </c>
+      <c r="BE3">
+        <v>1.34</v>
+      </c>
+      <c r="BF3">
+        <v>1.34</v>
+      </c>
+      <c r="BG3">
+        <v>1.34</v>
+      </c>
+      <c r="BH3">
+        <v>1.34</v>
+      </c>
+      <c r="BI3">
+        <v>1.34</v>
+      </c>
+      <c r="BJ3">
+        <v>1.34</v>
+      </c>
+      <c r="BK3">
+        <v>1.34</v>
+      </c>
+      <c r="BL3">
+        <v>1.34</v>
+      </c>
+      <c r="BM3">
+        <v>1.34</v>
+      </c>
+      <c r="BN3">
+        <v>1.34</v>
+      </c>
+      <c r="BO3">
+        <v>1.34</v>
+      </c>
+      <c r="BP3">
+        <v>1.34</v>
+      </c>
+      <c r="BQ3">
+        <v>1.34</v>
+      </c>
+      <c r="BR3">
+        <v>1.34</v>
+      </c>
+      <c r="BS3">
+        <v>1.34</v>
+      </c>
+      <c r="BT3">
+        <v>1.34</v>
+      </c>
+      <c r="BU3">
+        <v>1.34</v>
+      </c>
+      <c r="BV3">
+        <v>1.34</v>
+      </c>
+      <c r="BW3">
+        <v>1.34</v>
+      </c>
+      <c r="BX3">
+        <v>1.34</v>
+      </c>
+      <c r="BY3">
+        <v>1.34</v>
+      </c>
+      <c r="BZ3">
+        <v>1.34</v>
+      </c>
+      <c r="CA3">
+        <v>1.34</v>
+      </c>
+      <c r="CB3">
+        <v>1.34</v>
+      </c>
+      <c r="CC3">
+        <v>1.34</v>
+      </c>
+      <c r="CD3">
+        <v>1.34</v>
+      </c>
+      <c r="CE3">
+        <v>1.34</v>
+      </c>
+      <c r="CF3">
+        <v>1.34</v>
+      </c>
+      <c r="CG3">
+        <v>1.34</v>
+      </c>
+      <c r="CH3">
+        <v>1.34</v>
+      </c>
+      <c r="CI3">
+        <v>1.34</v>
+      </c>
+      <c r="CJ3">
+        <v>1.34</v>
+      </c>
+      <c r="CK3">
+        <v>1.34</v>
+      </c>
+      <c r="CL3">
+        <v>1.34</v>
+      </c>
+      <c r="CM3">
+        <v>1.34</v>
+      </c>
+      <c r="CN3">
+        <v>1.34</v>
+      </c>
+      <c r="CO3">
+        <v>1.34</v>
+      </c>
+      <c r="CP3">
+        <v>1.34</v>
+      </c>
+      <c r="CQ3">
+        <v>1.34</v>
+      </c>
+      <c r="CR3">
+        <v>1.34</v>
+      </c>
+      <c r="CS3">
+        <v>1.34</v>
+      </c>
+      <c r="CT3">
+        <v>1.34</v>
+      </c>
+      <c r="CU3">
+        <v>1.34</v>
+      </c>
+      <c r="CV3">
+        <v>1.34</v>
+      </c>
+      <c r="CW3">
+        <v>1.34</v>
+      </c>
+      <c r="CX3">
+        <v>1.34</v>
+      </c>
+      <c r="CY3">
+        <v>1.34</v>
+      </c>
+      <c r="CZ3">
+        <v>1.34</v>
+      </c>
+      <c r="DA3">
+        <v>1.34</v>
+      </c>
+      <c r="DB3">
+        <v>1.34</v>
+      </c>
+      <c r="DC3">
+        <v>1.34</v>
+      </c>
+      <c r="DD3">
+        <v>1.34</v>
+      </c>
+      <c r="DE3">
+        <v>1.34</v>
+      </c>
+      <c r="DF3">
+        <v>1.34</v>
+      </c>
+      <c r="DG3">
+        <v>1.34</v>
+      </c>
+      <c r="DH3">
+        <v>1.34</v>
+      </c>
+      <c r="DI3">
+        <v>1.34</v>
+      </c>
+      <c r="DJ3">
+        <v>1.34</v>
+      </c>
+      <c r="DK3">
+        <v>1.34</v>
+      </c>
+      <c r="DL3">
+        <v>1.34</v>
+      </c>
+      <c r="DM3">
+        <v>1.34</v>
+      </c>
+      <c r="DN3">
+        <v>1.34</v>
+      </c>
+      <c r="DO3">
+        <v>1.34</v>
+      </c>
+      <c r="DP3">
+        <v>1.34</v>
+      </c>
+      <c r="DQ3">
+        <v>1.34</v>
+      </c>
+      <c r="DR3">
+        <v>1.34</v>
+      </c>
+      <c r="DS3">
+        <v>1.34</v>
+      </c>
+      <c r="DT3">
+        <v>1.34</v>
+      </c>
+      <c r="DU3">
+        <v>1.34</v>
+      </c>
+      <c r="DV3">
+        <v>1.34</v>
+      </c>
+      <c r="DW3">
+        <v>1.34</v>
+      </c>
+      <c r="DX3">
+        <v>1.34</v>
+      </c>
+      <c r="DY3">
+        <v>1.34</v>
+      </c>
+      <c r="DZ3">
+        <v>1.34</v>
+      </c>
+      <c r="EA3">
+        <v>1.34</v>
+      </c>
+      <c r="EB3">
+        <v>1.34</v>
+      </c>
+      <c r="EC3">
+        <v>1.34</v>
+      </c>
+      <c r="ED3">
+        <v>1.34</v>
+      </c>
+      <c r="EE3">
+        <v>1.34</v>
+      </c>
+      <c r="EF3">
+        <v>1.34</v>
+      </c>
+      <c r="EG3">
+        <v>1.34</v>
+      </c>
+      <c r="EH3">
+        <v>1.34</v>
+      </c>
+      <c r="EI3">
+        <v>1.34</v>
+      </c>
+      <c r="EJ3">
+        <v>1.34</v>
+      </c>
+      <c r="EK3">
+        <v>1.34</v>
+      </c>
+      <c r="EL3">
+        <v>1.34</v>
+      </c>
+      <c r="EM3">
+        <v>1.34</v>
+      </c>
+      <c r="EN3">
+        <v>1.34</v>
+      </c>
+      <c r="EO3">
+        <v>1.34</v>
+      </c>
+      <c r="EP3">
+        <v>1.34</v>
+      </c>
+      <c r="EQ3">
+        <v>1.34</v>
+      </c>
+      <c r="ER3">
+        <v>1.34</v>
+      </c>
+      <c r="ES3">
+        <v>1.34</v>
+      </c>
+      <c r="ET3">
+        <v>1.34</v>
+      </c>
+      <c r="EU3">
+        <v>1.34</v>
+      </c>
+      <c r="EV3">
+        <v>1.34</v>
+      </c>
+      <c r="EW3">
+        <v>1.34</v>
+      </c>
+      <c r="EX3">
+        <v>1.34</v>
+      </c>
+      <c r="EY3">
+        <v>1.34</v>
+      </c>
+      <c r="EZ3">
+        <v>1.34</v>
+      </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1116,8 +2547,338 @@
       <c r="AT4">
         <v>1</v>
       </c>
+      <c r="AU4">
+        <v>1</v>
+      </c>
+      <c r="AV4">
+        <v>1</v>
+      </c>
+      <c r="AW4">
+        <v>1</v>
+      </c>
+      <c r="AX4">
+        <v>1</v>
+      </c>
+      <c r="AY4">
+        <v>1</v>
+      </c>
+      <c r="AZ4">
+        <v>1</v>
+      </c>
+      <c r="BA4">
+        <v>1</v>
+      </c>
+      <c r="BB4">
+        <v>1</v>
+      </c>
+      <c r="BC4">
+        <v>1</v>
+      </c>
+      <c r="BD4">
+        <v>1</v>
+      </c>
+      <c r="BE4">
+        <v>1</v>
+      </c>
+      <c r="BF4">
+        <v>1</v>
+      </c>
+      <c r="BG4">
+        <v>1</v>
+      </c>
+      <c r="BH4">
+        <v>1</v>
+      </c>
+      <c r="BI4">
+        <v>1</v>
+      </c>
+      <c r="BJ4">
+        <v>1</v>
+      </c>
+      <c r="BK4">
+        <v>1</v>
+      </c>
+      <c r="BL4">
+        <v>1</v>
+      </c>
+      <c r="BM4">
+        <v>1</v>
+      </c>
+      <c r="BN4">
+        <v>1</v>
+      </c>
+      <c r="BO4">
+        <v>1</v>
+      </c>
+      <c r="BP4">
+        <v>1</v>
+      </c>
+      <c r="BQ4">
+        <v>1</v>
+      </c>
+      <c r="BR4">
+        <v>1</v>
+      </c>
+      <c r="BS4">
+        <v>1</v>
+      </c>
+      <c r="BT4">
+        <v>1</v>
+      </c>
+      <c r="BU4">
+        <v>1</v>
+      </c>
+      <c r="BV4">
+        <v>1</v>
+      </c>
+      <c r="BW4">
+        <v>1</v>
+      </c>
+      <c r="BX4">
+        <v>1</v>
+      </c>
+      <c r="BY4">
+        <v>1</v>
+      </c>
+      <c r="BZ4">
+        <v>1</v>
+      </c>
+      <c r="CA4">
+        <v>1</v>
+      </c>
+      <c r="CB4">
+        <v>1</v>
+      </c>
+      <c r="CC4">
+        <v>1</v>
+      </c>
+      <c r="CD4">
+        <v>1</v>
+      </c>
+      <c r="CE4">
+        <v>1</v>
+      </c>
+      <c r="CF4">
+        <v>1</v>
+      </c>
+      <c r="CG4">
+        <v>1</v>
+      </c>
+      <c r="CH4">
+        <v>1</v>
+      </c>
+      <c r="CI4">
+        <v>1</v>
+      </c>
+      <c r="CJ4">
+        <v>1</v>
+      </c>
+      <c r="CK4">
+        <v>1</v>
+      </c>
+      <c r="CL4">
+        <v>1</v>
+      </c>
+      <c r="CM4">
+        <v>1</v>
+      </c>
+      <c r="CN4">
+        <v>1</v>
+      </c>
+      <c r="CO4">
+        <v>1</v>
+      </c>
+      <c r="CP4">
+        <v>1</v>
+      </c>
+      <c r="CQ4">
+        <v>1</v>
+      </c>
+      <c r="CR4">
+        <v>1</v>
+      </c>
+      <c r="CS4">
+        <v>1</v>
+      </c>
+      <c r="CT4">
+        <v>1</v>
+      </c>
+      <c r="CU4">
+        <v>1</v>
+      </c>
+      <c r="CV4">
+        <v>1</v>
+      </c>
+      <c r="CW4">
+        <v>1</v>
+      </c>
+      <c r="CX4">
+        <v>1</v>
+      </c>
+      <c r="CY4">
+        <v>1</v>
+      </c>
+      <c r="CZ4">
+        <v>1</v>
+      </c>
+      <c r="DA4">
+        <v>1</v>
+      </c>
+      <c r="DB4">
+        <v>1</v>
+      </c>
+      <c r="DC4">
+        <v>1</v>
+      </c>
+      <c r="DD4">
+        <v>1</v>
+      </c>
+      <c r="DE4">
+        <v>1</v>
+      </c>
+      <c r="DF4">
+        <v>1</v>
+      </c>
+      <c r="DG4">
+        <v>1</v>
+      </c>
+      <c r="DH4">
+        <v>1</v>
+      </c>
+      <c r="DI4">
+        <v>1</v>
+      </c>
+      <c r="DJ4">
+        <v>1</v>
+      </c>
+      <c r="DK4">
+        <v>1</v>
+      </c>
+      <c r="DL4">
+        <v>1</v>
+      </c>
+      <c r="DM4">
+        <v>1</v>
+      </c>
+      <c r="DN4">
+        <v>1</v>
+      </c>
+      <c r="DO4">
+        <v>1</v>
+      </c>
+      <c r="DP4">
+        <v>1</v>
+      </c>
+      <c r="DQ4">
+        <v>1</v>
+      </c>
+      <c r="DR4">
+        <v>1</v>
+      </c>
+      <c r="DS4">
+        <v>1</v>
+      </c>
+      <c r="DT4">
+        <v>1</v>
+      </c>
+      <c r="DU4">
+        <v>1</v>
+      </c>
+      <c r="DV4">
+        <v>1</v>
+      </c>
+      <c r="DW4">
+        <v>1</v>
+      </c>
+      <c r="DX4">
+        <v>1</v>
+      </c>
+      <c r="DY4">
+        <v>1</v>
+      </c>
+      <c r="DZ4">
+        <v>1</v>
+      </c>
+      <c r="EA4">
+        <v>1</v>
+      </c>
+      <c r="EB4">
+        <v>1</v>
+      </c>
+      <c r="EC4">
+        <v>1</v>
+      </c>
+      <c r="ED4">
+        <v>1</v>
+      </c>
+      <c r="EE4">
+        <v>1</v>
+      </c>
+      <c r="EF4">
+        <v>1</v>
+      </c>
+      <c r="EG4">
+        <v>1</v>
+      </c>
+      <c r="EH4">
+        <v>1</v>
+      </c>
+      <c r="EI4">
+        <v>1</v>
+      </c>
+      <c r="EJ4">
+        <v>1</v>
+      </c>
+      <c r="EK4">
+        <v>1</v>
+      </c>
+      <c r="EL4">
+        <v>1</v>
+      </c>
+      <c r="EM4">
+        <v>1</v>
+      </c>
+      <c r="EN4">
+        <v>1</v>
+      </c>
+      <c r="EO4">
+        <v>1</v>
+      </c>
+      <c r="EP4">
+        <v>1</v>
+      </c>
+      <c r="EQ4">
+        <v>1</v>
+      </c>
+      <c r="ER4">
+        <v>1</v>
+      </c>
+      <c r="ES4">
+        <v>1</v>
+      </c>
+      <c r="ET4">
+        <v>1</v>
+      </c>
+      <c r="EU4">
+        <v>1</v>
+      </c>
+      <c r="EV4">
+        <v>1</v>
+      </c>
+      <c r="EW4">
+        <v>1</v>
+      </c>
+      <c r="EX4">
+        <v>1</v>
+      </c>
+      <c r="EY4">
+        <v>1</v>
+      </c>
+      <c r="EZ4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -1256,8 +3017,338 @@
       <c r="AT5">
         <v>6.93</v>
       </c>
+      <c r="AU5">
+        <v>6.93</v>
+      </c>
+      <c r="AV5">
+        <v>6.93</v>
+      </c>
+      <c r="AW5">
+        <v>6.93</v>
+      </c>
+      <c r="AX5">
+        <v>6.93</v>
+      </c>
+      <c r="AY5">
+        <v>6.93</v>
+      </c>
+      <c r="AZ5">
+        <v>6.93</v>
+      </c>
+      <c r="BA5">
+        <v>6.93</v>
+      </c>
+      <c r="BB5">
+        <v>6.93</v>
+      </c>
+      <c r="BC5">
+        <v>6.93</v>
+      </c>
+      <c r="BD5">
+        <v>6.93</v>
+      </c>
+      <c r="BE5">
+        <v>6.93</v>
+      </c>
+      <c r="BF5">
+        <v>6.93</v>
+      </c>
+      <c r="BG5">
+        <v>6.93</v>
+      </c>
+      <c r="BH5">
+        <v>6.93</v>
+      </c>
+      <c r="BI5">
+        <v>6.93</v>
+      </c>
+      <c r="BJ5">
+        <v>6.93</v>
+      </c>
+      <c r="BK5">
+        <v>6.93</v>
+      </c>
+      <c r="BL5">
+        <v>6.93</v>
+      </c>
+      <c r="BM5">
+        <v>6.93</v>
+      </c>
+      <c r="BN5">
+        <v>6.93</v>
+      </c>
+      <c r="BO5">
+        <v>6.93</v>
+      </c>
+      <c r="BP5">
+        <v>6.93</v>
+      </c>
+      <c r="BQ5">
+        <v>6.93</v>
+      </c>
+      <c r="BR5">
+        <v>6.93</v>
+      </c>
+      <c r="BS5">
+        <v>6.93</v>
+      </c>
+      <c r="BT5">
+        <v>6.93</v>
+      </c>
+      <c r="BU5">
+        <v>6.93</v>
+      </c>
+      <c r="BV5">
+        <v>6.93</v>
+      </c>
+      <c r="BW5">
+        <v>6.93</v>
+      </c>
+      <c r="BX5">
+        <v>6.93</v>
+      </c>
+      <c r="BY5">
+        <v>6.93</v>
+      </c>
+      <c r="BZ5">
+        <v>6.93</v>
+      </c>
+      <c r="CA5">
+        <v>6.93</v>
+      </c>
+      <c r="CB5">
+        <v>6.93</v>
+      </c>
+      <c r="CC5">
+        <v>6.93</v>
+      </c>
+      <c r="CD5">
+        <v>6.93</v>
+      </c>
+      <c r="CE5">
+        <v>6.93</v>
+      </c>
+      <c r="CF5">
+        <v>6.93</v>
+      </c>
+      <c r="CG5">
+        <v>6.93</v>
+      </c>
+      <c r="CH5">
+        <v>6.93</v>
+      </c>
+      <c r="CI5">
+        <v>6.93</v>
+      </c>
+      <c r="CJ5">
+        <v>6.93</v>
+      </c>
+      <c r="CK5">
+        <v>6.93</v>
+      </c>
+      <c r="CL5">
+        <v>6.93</v>
+      </c>
+      <c r="CM5">
+        <v>6.93</v>
+      </c>
+      <c r="CN5">
+        <v>6.93</v>
+      </c>
+      <c r="CO5">
+        <v>6.93</v>
+      </c>
+      <c r="CP5">
+        <v>6.93</v>
+      </c>
+      <c r="CQ5">
+        <v>6.93</v>
+      </c>
+      <c r="CR5">
+        <v>6.93</v>
+      </c>
+      <c r="CS5">
+        <v>6.93</v>
+      </c>
+      <c r="CT5">
+        <v>6.93</v>
+      </c>
+      <c r="CU5">
+        <v>6.93</v>
+      </c>
+      <c r="CV5">
+        <v>6.93</v>
+      </c>
+      <c r="CW5">
+        <v>6.93</v>
+      </c>
+      <c r="CX5">
+        <v>6.93</v>
+      </c>
+      <c r="CY5">
+        <v>6.93</v>
+      </c>
+      <c r="CZ5">
+        <v>6.93</v>
+      </c>
+      <c r="DA5">
+        <v>6.93</v>
+      </c>
+      <c r="DB5">
+        <v>6.93</v>
+      </c>
+      <c r="DC5">
+        <v>6.93</v>
+      </c>
+      <c r="DD5">
+        <v>6.93</v>
+      </c>
+      <c r="DE5">
+        <v>6.93</v>
+      </c>
+      <c r="DF5">
+        <v>6.93</v>
+      </c>
+      <c r="DG5">
+        <v>6.93</v>
+      </c>
+      <c r="DH5">
+        <v>6.93</v>
+      </c>
+      <c r="DI5">
+        <v>6.93</v>
+      </c>
+      <c r="DJ5">
+        <v>6.93</v>
+      </c>
+      <c r="DK5">
+        <v>6.93</v>
+      </c>
+      <c r="DL5">
+        <v>6.93</v>
+      </c>
+      <c r="DM5">
+        <v>6.93</v>
+      </c>
+      <c r="DN5">
+        <v>6.93</v>
+      </c>
+      <c r="DO5">
+        <v>6.93</v>
+      </c>
+      <c r="DP5">
+        <v>6.93</v>
+      </c>
+      <c r="DQ5">
+        <v>6.93</v>
+      </c>
+      <c r="DR5">
+        <v>6.93</v>
+      </c>
+      <c r="DS5">
+        <v>6.93</v>
+      </c>
+      <c r="DT5">
+        <v>6.93</v>
+      </c>
+      <c r="DU5">
+        <v>6.93</v>
+      </c>
+      <c r="DV5">
+        <v>6.93</v>
+      </c>
+      <c r="DW5">
+        <v>6.93</v>
+      </c>
+      <c r="DX5">
+        <v>6.93</v>
+      </c>
+      <c r="DY5">
+        <v>6.93</v>
+      </c>
+      <c r="DZ5">
+        <v>6.93</v>
+      </c>
+      <c r="EA5">
+        <v>6.93</v>
+      </c>
+      <c r="EB5">
+        <v>6.93</v>
+      </c>
+      <c r="EC5">
+        <v>6.93</v>
+      </c>
+      <c r="ED5">
+        <v>6.93</v>
+      </c>
+      <c r="EE5">
+        <v>6.93</v>
+      </c>
+      <c r="EF5">
+        <v>6.93</v>
+      </c>
+      <c r="EG5">
+        <v>6.93</v>
+      </c>
+      <c r="EH5">
+        <v>6.93</v>
+      </c>
+      <c r="EI5">
+        <v>6.93</v>
+      </c>
+      <c r="EJ5">
+        <v>6.93</v>
+      </c>
+      <c r="EK5">
+        <v>6.93</v>
+      </c>
+      <c r="EL5">
+        <v>6.93</v>
+      </c>
+      <c r="EM5">
+        <v>6.93</v>
+      </c>
+      <c r="EN5">
+        <v>6.93</v>
+      </c>
+      <c r="EO5">
+        <v>6.93</v>
+      </c>
+      <c r="EP5">
+        <v>6.93</v>
+      </c>
+      <c r="EQ5">
+        <v>6.93</v>
+      </c>
+      <c r="ER5">
+        <v>6.93</v>
+      </c>
+      <c r="ES5">
+        <v>6.93</v>
+      </c>
+      <c r="ET5">
+        <v>6.93</v>
+      </c>
+      <c r="EU5">
+        <v>6.93</v>
+      </c>
+      <c r="EV5">
+        <v>6.93</v>
+      </c>
+      <c r="EW5">
+        <v>6.93</v>
+      </c>
+      <c r="EX5">
+        <v>6.93</v>
+      </c>
+      <c r="EY5">
+        <v>6.93</v>
+      </c>
+      <c r="EZ5">
+        <v>6.93</v>
+      </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -1396,8 +3487,338 @@
       <c r="AT6">
         <v>1</v>
       </c>
+      <c r="AU6">
+        <v>1</v>
+      </c>
+      <c r="AV6">
+        <v>1</v>
+      </c>
+      <c r="AW6">
+        <v>1</v>
+      </c>
+      <c r="AX6">
+        <v>1</v>
+      </c>
+      <c r="AY6">
+        <v>1</v>
+      </c>
+      <c r="AZ6">
+        <v>1</v>
+      </c>
+      <c r="BA6">
+        <v>1</v>
+      </c>
+      <c r="BB6">
+        <v>1</v>
+      </c>
+      <c r="BC6">
+        <v>1</v>
+      </c>
+      <c r="BD6">
+        <v>1</v>
+      </c>
+      <c r="BE6">
+        <v>1</v>
+      </c>
+      <c r="BF6">
+        <v>1</v>
+      </c>
+      <c r="BG6">
+        <v>1</v>
+      </c>
+      <c r="BH6">
+        <v>1</v>
+      </c>
+      <c r="BI6">
+        <v>1</v>
+      </c>
+      <c r="BJ6">
+        <v>1</v>
+      </c>
+      <c r="BK6">
+        <v>1</v>
+      </c>
+      <c r="BL6">
+        <v>1</v>
+      </c>
+      <c r="BM6">
+        <v>1</v>
+      </c>
+      <c r="BN6">
+        <v>1</v>
+      </c>
+      <c r="BO6">
+        <v>1</v>
+      </c>
+      <c r="BP6">
+        <v>1</v>
+      </c>
+      <c r="BQ6">
+        <v>1</v>
+      </c>
+      <c r="BR6">
+        <v>1</v>
+      </c>
+      <c r="BS6">
+        <v>1</v>
+      </c>
+      <c r="BT6">
+        <v>1</v>
+      </c>
+      <c r="BU6">
+        <v>1</v>
+      </c>
+      <c r="BV6">
+        <v>1</v>
+      </c>
+      <c r="BW6">
+        <v>1</v>
+      </c>
+      <c r="BX6">
+        <v>1</v>
+      </c>
+      <c r="BY6">
+        <v>1</v>
+      </c>
+      <c r="BZ6">
+        <v>1</v>
+      </c>
+      <c r="CA6">
+        <v>1</v>
+      </c>
+      <c r="CB6">
+        <v>1</v>
+      </c>
+      <c r="CC6">
+        <v>1</v>
+      </c>
+      <c r="CD6">
+        <v>1</v>
+      </c>
+      <c r="CE6">
+        <v>1</v>
+      </c>
+      <c r="CF6">
+        <v>1</v>
+      </c>
+      <c r="CG6">
+        <v>1</v>
+      </c>
+      <c r="CH6">
+        <v>1</v>
+      </c>
+      <c r="CI6">
+        <v>1</v>
+      </c>
+      <c r="CJ6">
+        <v>1</v>
+      </c>
+      <c r="CK6">
+        <v>1</v>
+      </c>
+      <c r="CL6">
+        <v>1</v>
+      </c>
+      <c r="CM6">
+        <v>1</v>
+      </c>
+      <c r="CN6">
+        <v>1</v>
+      </c>
+      <c r="CO6">
+        <v>1</v>
+      </c>
+      <c r="CP6">
+        <v>1</v>
+      </c>
+      <c r="CQ6">
+        <v>1</v>
+      </c>
+      <c r="CR6">
+        <v>1</v>
+      </c>
+      <c r="CS6">
+        <v>1</v>
+      </c>
+      <c r="CT6">
+        <v>1</v>
+      </c>
+      <c r="CU6">
+        <v>1</v>
+      </c>
+      <c r="CV6">
+        <v>1</v>
+      </c>
+      <c r="CW6">
+        <v>1</v>
+      </c>
+      <c r="CX6">
+        <v>1</v>
+      </c>
+      <c r="CY6">
+        <v>1</v>
+      </c>
+      <c r="CZ6">
+        <v>1</v>
+      </c>
+      <c r="DA6">
+        <v>1</v>
+      </c>
+      <c r="DB6">
+        <v>1</v>
+      </c>
+      <c r="DC6">
+        <v>1</v>
+      </c>
+      <c r="DD6">
+        <v>1</v>
+      </c>
+      <c r="DE6">
+        <v>1</v>
+      </c>
+      <c r="DF6">
+        <v>1</v>
+      </c>
+      <c r="DG6">
+        <v>1</v>
+      </c>
+      <c r="DH6">
+        <v>1</v>
+      </c>
+      <c r="DI6">
+        <v>1</v>
+      </c>
+      <c r="DJ6">
+        <v>1</v>
+      </c>
+      <c r="DK6">
+        <v>1</v>
+      </c>
+      <c r="DL6">
+        <v>1</v>
+      </c>
+      <c r="DM6">
+        <v>1</v>
+      </c>
+      <c r="DN6">
+        <v>1</v>
+      </c>
+      <c r="DO6">
+        <v>1</v>
+      </c>
+      <c r="DP6">
+        <v>1</v>
+      </c>
+      <c r="DQ6">
+        <v>1</v>
+      </c>
+      <c r="DR6">
+        <v>1</v>
+      </c>
+      <c r="DS6">
+        <v>1</v>
+      </c>
+      <c r="DT6">
+        <v>1</v>
+      </c>
+      <c r="DU6">
+        <v>1</v>
+      </c>
+      <c r="DV6">
+        <v>1</v>
+      </c>
+      <c r="DW6">
+        <v>1</v>
+      </c>
+      <c r="DX6">
+        <v>1</v>
+      </c>
+      <c r="DY6">
+        <v>1</v>
+      </c>
+      <c r="DZ6">
+        <v>1</v>
+      </c>
+      <c r="EA6">
+        <v>1</v>
+      </c>
+      <c r="EB6">
+        <v>1</v>
+      </c>
+      <c r="EC6">
+        <v>1</v>
+      </c>
+      <c r="ED6">
+        <v>1</v>
+      </c>
+      <c r="EE6">
+        <v>1</v>
+      </c>
+      <c r="EF6">
+        <v>1</v>
+      </c>
+      <c r="EG6">
+        <v>1</v>
+      </c>
+      <c r="EH6">
+        <v>1</v>
+      </c>
+      <c r="EI6">
+        <v>1</v>
+      </c>
+      <c r="EJ6">
+        <v>1</v>
+      </c>
+      <c r="EK6">
+        <v>1</v>
+      </c>
+      <c r="EL6">
+        <v>1</v>
+      </c>
+      <c r="EM6">
+        <v>1</v>
+      </c>
+      <c r="EN6">
+        <v>1</v>
+      </c>
+      <c r="EO6">
+        <v>1</v>
+      </c>
+      <c r="EP6">
+        <v>1</v>
+      </c>
+      <c r="EQ6">
+        <v>1</v>
+      </c>
+      <c r="ER6">
+        <v>1</v>
+      </c>
+      <c r="ES6">
+        <v>1</v>
+      </c>
+      <c r="ET6">
+        <v>1</v>
+      </c>
+      <c r="EU6">
+        <v>1</v>
+      </c>
+      <c r="EV6">
+        <v>1</v>
+      </c>
+      <c r="EW6">
+        <v>1</v>
+      </c>
+      <c r="EX6">
+        <v>1</v>
+      </c>
+      <c r="EY6">
+        <v>1</v>
+      </c>
+      <c r="EZ6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1536,8 +3957,338 @@
       <c r="AT7">
         <v>0.13</v>
       </c>
+      <c r="AU7">
+        <v>0.13</v>
+      </c>
+      <c r="AV7">
+        <v>0.13</v>
+      </c>
+      <c r="AW7">
+        <v>0.13</v>
+      </c>
+      <c r="AX7">
+        <v>0.13</v>
+      </c>
+      <c r="AY7">
+        <v>0.13</v>
+      </c>
+      <c r="AZ7">
+        <v>0.13</v>
+      </c>
+      <c r="BA7">
+        <v>0.13</v>
+      </c>
+      <c r="BB7">
+        <v>0.13</v>
+      </c>
+      <c r="BC7">
+        <v>0.13</v>
+      </c>
+      <c r="BD7">
+        <v>0.13</v>
+      </c>
+      <c r="BE7">
+        <v>0.13</v>
+      </c>
+      <c r="BF7">
+        <v>0.13</v>
+      </c>
+      <c r="BG7">
+        <v>0.13</v>
+      </c>
+      <c r="BH7">
+        <v>0.13</v>
+      </c>
+      <c r="BI7">
+        <v>0.13</v>
+      </c>
+      <c r="BJ7">
+        <v>0.13</v>
+      </c>
+      <c r="BK7">
+        <v>0.13</v>
+      </c>
+      <c r="BL7">
+        <v>0.13</v>
+      </c>
+      <c r="BM7">
+        <v>0.13</v>
+      </c>
+      <c r="BN7">
+        <v>0.13</v>
+      </c>
+      <c r="BO7">
+        <v>0.13</v>
+      </c>
+      <c r="BP7">
+        <v>0.13</v>
+      </c>
+      <c r="BQ7">
+        <v>0.13</v>
+      </c>
+      <c r="BR7">
+        <v>0.13</v>
+      </c>
+      <c r="BS7">
+        <v>0.13</v>
+      </c>
+      <c r="BT7">
+        <v>0.13</v>
+      </c>
+      <c r="BU7">
+        <v>0.13</v>
+      </c>
+      <c r="BV7">
+        <v>0.13</v>
+      </c>
+      <c r="BW7">
+        <v>0.13</v>
+      </c>
+      <c r="BX7">
+        <v>0.13</v>
+      </c>
+      <c r="BY7">
+        <v>0.13</v>
+      </c>
+      <c r="BZ7">
+        <v>0.13</v>
+      </c>
+      <c r="CA7">
+        <v>0.13</v>
+      </c>
+      <c r="CB7">
+        <v>0.13</v>
+      </c>
+      <c r="CC7">
+        <v>0.13</v>
+      </c>
+      <c r="CD7">
+        <v>0.13</v>
+      </c>
+      <c r="CE7">
+        <v>0.13</v>
+      </c>
+      <c r="CF7">
+        <v>0.13</v>
+      </c>
+      <c r="CG7">
+        <v>0.13</v>
+      </c>
+      <c r="CH7">
+        <v>0.13</v>
+      </c>
+      <c r="CI7">
+        <v>0.13</v>
+      </c>
+      <c r="CJ7">
+        <v>0.13</v>
+      </c>
+      <c r="CK7">
+        <v>0.13</v>
+      </c>
+      <c r="CL7">
+        <v>0.13</v>
+      </c>
+      <c r="CM7">
+        <v>0.13</v>
+      </c>
+      <c r="CN7">
+        <v>0.13</v>
+      </c>
+      <c r="CO7">
+        <v>0.13</v>
+      </c>
+      <c r="CP7">
+        <v>0.13</v>
+      </c>
+      <c r="CQ7">
+        <v>0.13</v>
+      </c>
+      <c r="CR7">
+        <v>0.13</v>
+      </c>
+      <c r="CS7">
+        <v>0.13</v>
+      </c>
+      <c r="CT7">
+        <v>0.13</v>
+      </c>
+      <c r="CU7">
+        <v>0.13</v>
+      </c>
+      <c r="CV7">
+        <v>0.13</v>
+      </c>
+      <c r="CW7">
+        <v>0.13</v>
+      </c>
+      <c r="CX7">
+        <v>0.13</v>
+      </c>
+      <c r="CY7">
+        <v>0.13</v>
+      </c>
+      <c r="CZ7">
+        <v>0.13</v>
+      </c>
+      <c r="DA7">
+        <v>0.13</v>
+      </c>
+      <c r="DB7">
+        <v>0.13</v>
+      </c>
+      <c r="DC7">
+        <v>0.13</v>
+      </c>
+      <c r="DD7">
+        <v>0.13</v>
+      </c>
+      <c r="DE7">
+        <v>0.13</v>
+      </c>
+      <c r="DF7">
+        <v>0.13</v>
+      </c>
+      <c r="DG7">
+        <v>0.13</v>
+      </c>
+      <c r="DH7">
+        <v>0.13</v>
+      </c>
+      <c r="DI7">
+        <v>0.13</v>
+      </c>
+      <c r="DJ7">
+        <v>0.13</v>
+      </c>
+      <c r="DK7">
+        <v>0.13</v>
+      </c>
+      <c r="DL7">
+        <v>0.13</v>
+      </c>
+      <c r="DM7">
+        <v>0.13</v>
+      </c>
+      <c r="DN7">
+        <v>0.13</v>
+      </c>
+      <c r="DO7">
+        <v>0.13</v>
+      </c>
+      <c r="DP7">
+        <v>0.13</v>
+      </c>
+      <c r="DQ7">
+        <v>0.13</v>
+      </c>
+      <c r="DR7">
+        <v>0.13</v>
+      </c>
+      <c r="DS7">
+        <v>0.13</v>
+      </c>
+      <c r="DT7">
+        <v>0.13</v>
+      </c>
+      <c r="DU7">
+        <v>0.13</v>
+      </c>
+      <c r="DV7">
+        <v>0.13</v>
+      </c>
+      <c r="DW7">
+        <v>0.13</v>
+      </c>
+      <c r="DX7">
+        <v>0.13</v>
+      </c>
+      <c r="DY7">
+        <v>0.13</v>
+      </c>
+      <c r="DZ7">
+        <v>0.13</v>
+      </c>
+      <c r="EA7">
+        <v>0.13</v>
+      </c>
+      <c r="EB7">
+        <v>0.13</v>
+      </c>
+      <c r="EC7">
+        <v>0.13</v>
+      </c>
+      <c r="ED7">
+        <v>0.13</v>
+      </c>
+      <c r="EE7">
+        <v>0.13</v>
+      </c>
+      <c r="EF7">
+        <v>0.13</v>
+      </c>
+      <c r="EG7">
+        <v>0.13</v>
+      </c>
+      <c r="EH7">
+        <v>0.13</v>
+      </c>
+      <c r="EI7">
+        <v>0.13</v>
+      </c>
+      <c r="EJ7">
+        <v>0.13</v>
+      </c>
+      <c r="EK7">
+        <v>0.13</v>
+      </c>
+      <c r="EL7">
+        <v>0.13</v>
+      </c>
+      <c r="EM7">
+        <v>0.13</v>
+      </c>
+      <c r="EN7">
+        <v>0.13</v>
+      </c>
+      <c r="EO7">
+        <v>0.13</v>
+      </c>
+      <c r="EP7">
+        <v>0.13</v>
+      </c>
+      <c r="EQ7">
+        <v>0.13</v>
+      </c>
+      <c r="ER7">
+        <v>0.13</v>
+      </c>
+      <c r="ES7">
+        <v>0.13</v>
+      </c>
+      <c r="ET7">
+        <v>0.13</v>
+      </c>
+      <c r="EU7">
+        <v>0.13</v>
+      </c>
+      <c r="EV7">
+        <v>0.13</v>
+      </c>
+      <c r="EW7">
+        <v>0.13</v>
+      </c>
+      <c r="EX7">
+        <v>0.13</v>
+      </c>
+      <c r="EY7">
+        <v>0.13</v>
+      </c>
+      <c r="EZ7">
+        <v>0.13</v>
+      </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1676,8 +4427,338 @@
       <c r="AT8">
         <v>1</v>
       </c>
+      <c r="AU8">
+        <v>1</v>
+      </c>
+      <c r="AV8">
+        <v>1</v>
+      </c>
+      <c r="AW8">
+        <v>1</v>
+      </c>
+      <c r="AX8">
+        <v>1</v>
+      </c>
+      <c r="AY8">
+        <v>1</v>
+      </c>
+      <c r="AZ8">
+        <v>1</v>
+      </c>
+      <c r="BA8">
+        <v>1</v>
+      </c>
+      <c r="BB8">
+        <v>1</v>
+      </c>
+      <c r="BC8">
+        <v>1</v>
+      </c>
+      <c r="BD8">
+        <v>1</v>
+      </c>
+      <c r="BE8">
+        <v>1</v>
+      </c>
+      <c r="BF8">
+        <v>1</v>
+      </c>
+      <c r="BG8">
+        <v>1</v>
+      </c>
+      <c r="BH8">
+        <v>1</v>
+      </c>
+      <c r="BI8">
+        <v>1</v>
+      </c>
+      <c r="BJ8">
+        <v>1</v>
+      </c>
+      <c r="BK8">
+        <v>1</v>
+      </c>
+      <c r="BL8">
+        <v>1</v>
+      </c>
+      <c r="BM8">
+        <v>1</v>
+      </c>
+      <c r="BN8">
+        <v>1</v>
+      </c>
+      <c r="BO8">
+        <v>1</v>
+      </c>
+      <c r="BP8">
+        <v>1</v>
+      </c>
+      <c r="BQ8">
+        <v>1</v>
+      </c>
+      <c r="BR8">
+        <v>1</v>
+      </c>
+      <c r="BS8">
+        <v>1</v>
+      </c>
+      <c r="BT8">
+        <v>1</v>
+      </c>
+      <c r="BU8">
+        <v>1</v>
+      </c>
+      <c r="BV8">
+        <v>1</v>
+      </c>
+      <c r="BW8">
+        <v>1</v>
+      </c>
+      <c r="BX8">
+        <v>1</v>
+      </c>
+      <c r="BY8">
+        <v>1</v>
+      </c>
+      <c r="BZ8">
+        <v>1</v>
+      </c>
+      <c r="CA8">
+        <v>1</v>
+      </c>
+      <c r="CB8">
+        <v>1</v>
+      </c>
+      <c r="CC8">
+        <v>1</v>
+      </c>
+      <c r="CD8">
+        <v>1</v>
+      </c>
+      <c r="CE8">
+        <v>1</v>
+      </c>
+      <c r="CF8">
+        <v>1</v>
+      </c>
+      <c r="CG8">
+        <v>1</v>
+      </c>
+      <c r="CH8">
+        <v>1</v>
+      </c>
+      <c r="CI8">
+        <v>1</v>
+      </c>
+      <c r="CJ8">
+        <v>1</v>
+      </c>
+      <c r="CK8">
+        <v>1</v>
+      </c>
+      <c r="CL8">
+        <v>1</v>
+      </c>
+      <c r="CM8">
+        <v>1</v>
+      </c>
+      <c r="CN8">
+        <v>1</v>
+      </c>
+      <c r="CO8">
+        <v>1</v>
+      </c>
+      <c r="CP8">
+        <v>1</v>
+      </c>
+      <c r="CQ8">
+        <v>1</v>
+      </c>
+      <c r="CR8">
+        <v>1</v>
+      </c>
+      <c r="CS8">
+        <v>1</v>
+      </c>
+      <c r="CT8">
+        <v>1</v>
+      </c>
+      <c r="CU8">
+        <v>1</v>
+      </c>
+      <c r="CV8">
+        <v>1</v>
+      </c>
+      <c r="CW8">
+        <v>1</v>
+      </c>
+      <c r="CX8">
+        <v>1</v>
+      </c>
+      <c r="CY8">
+        <v>1</v>
+      </c>
+      <c r="CZ8">
+        <v>1</v>
+      </c>
+      <c r="DA8">
+        <v>1</v>
+      </c>
+      <c r="DB8">
+        <v>1</v>
+      </c>
+      <c r="DC8">
+        <v>1</v>
+      </c>
+      <c r="DD8">
+        <v>1</v>
+      </c>
+      <c r="DE8">
+        <v>1</v>
+      </c>
+      <c r="DF8">
+        <v>1</v>
+      </c>
+      <c r="DG8">
+        <v>1</v>
+      </c>
+      <c r="DH8">
+        <v>1</v>
+      </c>
+      <c r="DI8">
+        <v>1</v>
+      </c>
+      <c r="DJ8">
+        <v>1</v>
+      </c>
+      <c r="DK8">
+        <v>1</v>
+      </c>
+      <c r="DL8">
+        <v>1</v>
+      </c>
+      <c r="DM8">
+        <v>1</v>
+      </c>
+      <c r="DN8">
+        <v>1</v>
+      </c>
+      <c r="DO8">
+        <v>1</v>
+      </c>
+      <c r="DP8">
+        <v>1</v>
+      </c>
+      <c r="DQ8">
+        <v>1</v>
+      </c>
+      <c r="DR8">
+        <v>1</v>
+      </c>
+      <c r="DS8">
+        <v>1</v>
+      </c>
+      <c r="DT8">
+        <v>1</v>
+      </c>
+      <c r="DU8">
+        <v>1</v>
+      </c>
+      <c r="DV8">
+        <v>1</v>
+      </c>
+      <c r="DW8">
+        <v>1</v>
+      </c>
+      <c r="DX8">
+        <v>1</v>
+      </c>
+      <c r="DY8">
+        <v>1</v>
+      </c>
+      <c r="DZ8">
+        <v>1</v>
+      </c>
+      <c r="EA8">
+        <v>1</v>
+      </c>
+      <c r="EB8">
+        <v>1</v>
+      </c>
+      <c r="EC8">
+        <v>1</v>
+      </c>
+      <c r="ED8">
+        <v>1</v>
+      </c>
+      <c r="EE8">
+        <v>1</v>
+      </c>
+      <c r="EF8">
+        <v>1</v>
+      </c>
+      <c r="EG8">
+        <v>1</v>
+      </c>
+      <c r="EH8">
+        <v>1</v>
+      </c>
+      <c r="EI8">
+        <v>1</v>
+      </c>
+      <c r="EJ8">
+        <v>1</v>
+      </c>
+      <c r="EK8">
+        <v>1</v>
+      </c>
+      <c r="EL8">
+        <v>1</v>
+      </c>
+      <c r="EM8">
+        <v>1</v>
+      </c>
+      <c r="EN8">
+        <v>1</v>
+      </c>
+      <c r="EO8">
+        <v>1</v>
+      </c>
+      <c r="EP8">
+        <v>1</v>
+      </c>
+      <c r="EQ8">
+        <v>1</v>
+      </c>
+      <c r="ER8">
+        <v>1</v>
+      </c>
+      <c r="ES8">
+        <v>1</v>
+      </c>
+      <c r="ET8">
+        <v>1</v>
+      </c>
+      <c r="EU8">
+        <v>1</v>
+      </c>
+      <c r="EV8">
+        <v>1</v>
+      </c>
+      <c r="EW8">
+        <v>1</v>
+      </c>
+      <c r="EX8">
+        <v>1</v>
+      </c>
+      <c r="EY8">
+        <v>1</v>
+      </c>
+      <c r="EZ8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1816,8 +4897,338 @@
       <c r="AT9">
         <v>0.19</v>
       </c>
+      <c r="AU9">
+        <v>0.19</v>
+      </c>
+      <c r="AV9">
+        <v>0.19</v>
+      </c>
+      <c r="AW9">
+        <v>0.19</v>
+      </c>
+      <c r="AX9">
+        <v>0.19</v>
+      </c>
+      <c r="AY9">
+        <v>0.19</v>
+      </c>
+      <c r="AZ9">
+        <v>0.19</v>
+      </c>
+      <c r="BA9">
+        <v>0.19</v>
+      </c>
+      <c r="BB9">
+        <v>0.19</v>
+      </c>
+      <c r="BC9">
+        <v>0.19</v>
+      </c>
+      <c r="BD9">
+        <v>0.19</v>
+      </c>
+      <c r="BE9">
+        <v>0.19</v>
+      </c>
+      <c r="BF9">
+        <v>0.19</v>
+      </c>
+      <c r="BG9">
+        <v>0.19</v>
+      </c>
+      <c r="BH9">
+        <v>0.19</v>
+      </c>
+      <c r="BI9">
+        <v>0.19</v>
+      </c>
+      <c r="BJ9">
+        <v>0.19</v>
+      </c>
+      <c r="BK9">
+        <v>0.19</v>
+      </c>
+      <c r="BL9">
+        <v>0.19</v>
+      </c>
+      <c r="BM9">
+        <v>0.19</v>
+      </c>
+      <c r="BN9">
+        <v>0.19</v>
+      </c>
+      <c r="BO9">
+        <v>0.19</v>
+      </c>
+      <c r="BP9">
+        <v>0.19</v>
+      </c>
+      <c r="BQ9">
+        <v>0.19</v>
+      </c>
+      <c r="BR9">
+        <v>0.19</v>
+      </c>
+      <c r="BS9">
+        <v>0.19</v>
+      </c>
+      <c r="BT9">
+        <v>0.19</v>
+      </c>
+      <c r="BU9">
+        <v>0.19</v>
+      </c>
+      <c r="BV9">
+        <v>0.19</v>
+      </c>
+      <c r="BW9">
+        <v>0.19</v>
+      </c>
+      <c r="BX9">
+        <v>0.19</v>
+      </c>
+      <c r="BY9">
+        <v>0.19</v>
+      </c>
+      <c r="BZ9">
+        <v>0.19</v>
+      </c>
+      <c r="CA9">
+        <v>0.19</v>
+      </c>
+      <c r="CB9">
+        <v>0.19</v>
+      </c>
+      <c r="CC9">
+        <v>0.19</v>
+      </c>
+      <c r="CD9">
+        <v>0.19</v>
+      </c>
+      <c r="CE9">
+        <v>0.19</v>
+      </c>
+      <c r="CF9">
+        <v>0.19</v>
+      </c>
+      <c r="CG9">
+        <v>0.19</v>
+      </c>
+      <c r="CH9">
+        <v>0.19</v>
+      </c>
+      <c r="CI9">
+        <v>0.19</v>
+      </c>
+      <c r="CJ9">
+        <v>0.19</v>
+      </c>
+      <c r="CK9">
+        <v>0.19</v>
+      </c>
+      <c r="CL9">
+        <v>0.19</v>
+      </c>
+      <c r="CM9">
+        <v>0.19</v>
+      </c>
+      <c r="CN9">
+        <v>0.19</v>
+      </c>
+      <c r="CO9">
+        <v>0.19</v>
+      </c>
+      <c r="CP9">
+        <v>0.19</v>
+      </c>
+      <c r="CQ9">
+        <v>0.19</v>
+      </c>
+      <c r="CR9">
+        <v>0.19</v>
+      </c>
+      <c r="CS9">
+        <v>0.19</v>
+      </c>
+      <c r="CT9">
+        <v>0.19</v>
+      </c>
+      <c r="CU9">
+        <v>0.19</v>
+      </c>
+      <c r="CV9">
+        <v>0.19</v>
+      </c>
+      <c r="CW9">
+        <v>0.19</v>
+      </c>
+      <c r="CX9">
+        <v>0.19</v>
+      </c>
+      <c r="CY9">
+        <v>0.19</v>
+      </c>
+      <c r="CZ9">
+        <v>0.19</v>
+      </c>
+      <c r="DA9">
+        <v>0.19</v>
+      </c>
+      <c r="DB9">
+        <v>0.19</v>
+      </c>
+      <c r="DC9">
+        <v>0.19</v>
+      </c>
+      <c r="DD9">
+        <v>0.19</v>
+      </c>
+      <c r="DE9">
+        <v>0.19</v>
+      </c>
+      <c r="DF9">
+        <v>0.19</v>
+      </c>
+      <c r="DG9">
+        <v>0.19</v>
+      </c>
+      <c r="DH9">
+        <v>0.19</v>
+      </c>
+      <c r="DI9">
+        <v>0.19</v>
+      </c>
+      <c r="DJ9">
+        <v>0.19</v>
+      </c>
+      <c r="DK9">
+        <v>0.19</v>
+      </c>
+      <c r="DL9">
+        <v>0.19</v>
+      </c>
+      <c r="DM9">
+        <v>0.19</v>
+      </c>
+      <c r="DN9">
+        <v>0.19</v>
+      </c>
+      <c r="DO9">
+        <v>0.19</v>
+      </c>
+      <c r="DP9">
+        <v>0.19</v>
+      </c>
+      <c r="DQ9">
+        <v>0.19</v>
+      </c>
+      <c r="DR9">
+        <v>0.19</v>
+      </c>
+      <c r="DS9">
+        <v>0.19</v>
+      </c>
+      <c r="DT9">
+        <v>0.19</v>
+      </c>
+      <c r="DU9">
+        <v>0.19</v>
+      </c>
+      <c r="DV9">
+        <v>0.19</v>
+      </c>
+      <c r="DW9">
+        <v>0.19</v>
+      </c>
+      <c r="DX9">
+        <v>0.19</v>
+      </c>
+      <c r="DY9">
+        <v>0.19</v>
+      </c>
+      <c r="DZ9">
+        <v>0.19</v>
+      </c>
+      <c r="EA9">
+        <v>0.19</v>
+      </c>
+      <c r="EB9">
+        <v>0.19</v>
+      </c>
+      <c r="EC9">
+        <v>0.19</v>
+      </c>
+      <c r="ED9">
+        <v>0.19</v>
+      </c>
+      <c r="EE9">
+        <v>0.19</v>
+      </c>
+      <c r="EF9">
+        <v>0.19</v>
+      </c>
+      <c r="EG9">
+        <v>0.19</v>
+      </c>
+      <c r="EH9">
+        <v>0.19</v>
+      </c>
+      <c r="EI9">
+        <v>0.19</v>
+      </c>
+      <c r="EJ9">
+        <v>0.19</v>
+      </c>
+      <c r="EK9">
+        <v>0.19</v>
+      </c>
+      <c r="EL9">
+        <v>0.19</v>
+      </c>
+      <c r="EM9">
+        <v>0.19</v>
+      </c>
+      <c r="EN9">
+        <v>0.19</v>
+      </c>
+      <c r="EO9">
+        <v>0.19</v>
+      </c>
+      <c r="EP9">
+        <v>0.19</v>
+      </c>
+      <c r="EQ9">
+        <v>0.19</v>
+      </c>
+      <c r="ER9">
+        <v>0.19</v>
+      </c>
+      <c r="ES9">
+        <v>0.19</v>
+      </c>
+      <c r="ET9">
+        <v>0.19</v>
+      </c>
+      <c r="EU9">
+        <v>0.19</v>
+      </c>
+      <c r="EV9">
+        <v>0.19</v>
+      </c>
+      <c r="EW9">
+        <v>0.19</v>
+      </c>
+      <c r="EX9">
+        <v>0.19</v>
+      </c>
+      <c r="EY9">
+        <v>0.19</v>
+      </c>
+      <c r="EZ9">
+        <v>0.19</v>
+      </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1956,8 +5367,338 @@
       <c r="AT10">
         <v>1</v>
       </c>
+      <c r="AU10">
+        <v>1</v>
+      </c>
+      <c r="AV10">
+        <v>1</v>
+      </c>
+      <c r="AW10">
+        <v>1</v>
+      </c>
+      <c r="AX10">
+        <v>1</v>
+      </c>
+      <c r="AY10">
+        <v>1</v>
+      </c>
+      <c r="AZ10">
+        <v>1</v>
+      </c>
+      <c r="BA10">
+        <v>1</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
+      <c r="BC10">
+        <v>1</v>
+      </c>
+      <c r="BD10">
+        <v>1</v>
+      </c>
+      <c r="BE10">
+        <v>1</v>
+      </c>
+      <c r="BF10">
+        <v>1</v>
+      </c>
+      <c r="BG10">
+        <v>1</v>
+      </c>
+      <c r="BH10">
+        <v>1</v>
+      </c>
+      <c r="BI10">
+        <v>1</v>
+      </c>
+      <c r="BJ10">
+        <v>1</v>
+      </c>
+      <c r="BK10">
+        <v>1</v>
+      </c>
+      <c r="BL10">
+        <v>1</v>
+      </c>
+      <c r="BM10">
+        <v>1</v>
+      </c>
+      <c r="BN10">
+        <v>1</v>
+      </c>
+      <c r="BO10">
+        <v>1</v>
+      </c>
+      <c r="BP10">
+        <v>1</v>
+      </c>
+      <c r="BQ10">
+        <v>1</v>
+      </c>
+      <c r="BR10">
+        <v>1</v>
+      </c>
+      <c r="BS10">
+        <v>1</v>
+      </c>
+      <c r="BT10">
+        <v>1</v>
+      </c>
+      <c r="BU10">
+        <v>1</v>
+      </c>
+      <c r="BV10">
+        <v>1</v>
+      </c>
+      <c r="BW10">
+        <v>1</v>
+      </c>
+      <c r="BX10">
+        <v>1</v>
+      </c>
+      <c r="BY10">
+        <v>1</v>
+      </c>
+      <c r="BZ10">
+        <v>1</v>
+      </c>
+      <c r="CA10">
+        <v>1</v>
+      </c>
+      <c r="CB10">
+        <v>1</v>
+      </c>
+      <c r="CC10">
+        <v>1</v>
+      </c>
+      <c r="CD10">
+        <v>1</v>
+      </c>
+      <c r="CE10">
+        <v>1</v>
+      </c>
+      <c r="CF10">
+        <v>1</v>
+      </c>
+      <c r="CG10">
+        <v>1</v>
+      </c>
+      <c r="CH10">
+        <v>1</v>
+      </c>
+      <c r="CI10">
+        <v>1</v>
+      </c>
+      <c r="CJ10">
+        <v>1</v>
+      </c>
+      <c r="CK10">
+        <v>1</v>
+      </c>
+      <c r="CL10">
+        <v>1</v>
+      </c>
+      <c r="CM10">
+        <v>1</v>
+      </c>
+      <c r="CN10">
+        <v>1</v>
+      </c>
+      <c r="CO10">
+        <v>1</v>
+      </c>
+      <c r="CP10">
+        <v>1</v>
+      </c>
+      <c r="CQ10">
+        <v>1</v>
+      </c>
+      <c r="CR10">
+        <v>1</v>
+      </c>
+      <c r="CS10">
+        <v>1</v>
+      </c>
+      <c r="CT10">
+        <v>1</v>
+      </c>
+      <c r="CU10">
+        <v>1</v>
+      </c>
+      <c r="CV10">
+        <v>1</v>
+      </c>
+      <c r="CW10">
+        <v>1</v>
+      </c>
+      <c r="CX10">
+        <v>1</v>
+      </c>
+      <c r="CY10">
+        <v>1</v>
+      </c>
+      <c r="CZ10">
+        <v>1</v>
+      </c>
+      <c r="DA10">
+        <v>1</v>
+      </c>
+      <c r="DB10">
+        <v>1</v>
+      </c>
+      <c r="DC10">
+        <v>1</v>
+      </c>
+      <c r="DD10">
+        <v>1</v>
+      </c>
+      <c r="DE10">
+        <v>1</v>
+      </c>
+      <c r="DF10">
+        <v>1</v>
+      </c>
+      <c r="DG10">
+        <v>1</v>
+      </c>
+      <c r="DH10">
+        <v>1</v>
+      </c>
+      <c r="DI10">
+        <v>1</v>
+      </c>
+      <c r="DJ10">
+        <v>1</v>
+      </c>
+      <c r="DK10">
+        <v>1</v>
+      </c>
+      <c r="DL10">
+        <v>1</v>
+      </c>
+      <c r="DM10">
+        <v>1</v>
+      </c>
+      <c r="DN10">
+        <v>1</v>
+      </c>
+      <c r="DO10">
+        <v>1</v>
+      </c>
+      <c r="DP10">
+        <v>1</v>
+      </c>
+      <c r="DQ10">
+        <v>1</v>
+      </c>
+      <c r="DR10">
+        <v>1</v>
+      </c>
+      <c r="DS10">
+        <v>1</v>
+      </c>
+      <c r="DT10">
+        <v>1</v>
+      </c>
+      <c r="DU10">
+        <v>1</v>
+      </c>
+      <c r="DV10">
+        <v>1</v>
+      </c>
+      <c r="DW10">
+        <v>1</v>
+      </c>
+      <c r="DX10">
+        <v>1</v>
+      </c>
+      <c r="DY10">
+        <v>1</v>
+      </c>
+      <c r="DZ10">
+        <v>1</v>
+      </c>
+      <c r="EA10">
+        <v>1</v>
+      </c>
+      <c r="EB10">
+        <v>1</v>
+      </c>
+      <c r="EC10">
+        <v>1</v>
+      </c>
+      <c r="ED10">
+        <v>1</v>
+      </c>
+      <c r="EE10">
+        <v>1</v>
+      </c>
+      <c r="EF10">
+        <v>1</v>
+      </c>
+      <c r="EG10">
+        <v>1</v>
+      </c>
+      <c r="EH10">
+        <v>1</v>
+      </c>
+      <c r="EI10">
+        <v>1</v>
+      </c>
+      <c r="EJ10">
+        <v>1</v>
+      </c>
+      <c r="EK10">
+        <v>1</v>
+      </c>
+      <c r="EL10">
+        <v>1</v>
+      </c>
+      <c r="EM10">
+        <v>1</v>
+      </c>
+      <c r="EN10">
+        <v>1</v>
+      </c>
+      <c r="EO10">
+        <v>1</v>
+      </c>
+      <c r="EP10">
+        <v>1</v>
+      </c>
+      <c r="EQ10">
+        <v>1</v>
+      </c>
+      <c r="ER10">
+        <v>1</v>
+      </c>
+      <c r="ES10">
+        <v>1</v>
+      </c>
+      <c r="ET10">
+        <v>1</v>
+      </c>
+      <c r="EU10">
+        <v>1</v>
+      </c>
+      <c r="EV10">
+        <v>1</v>
+      </c>
+      <c r="EW10">
+        <v>1</v>
+      </c>
+      <c r="EX10">
+        <v>1</v>
+      </c>
+      <c r="EY10">
+        <v>1</v>
+      </c>
+      <c r="EZ10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2094,6 +5835,336 @@
         <v>0.48</v>
       </c>
       <c r="AT11">
+        <v>0.48</v>
+      </c>
+      <c r="AU11">
+        <v>0.48</v>
+      </c>
+      <c r="AV11">
+        <v>0.48</v>
+      </c>
+      <c r="AW11">
+        <v>0.48</v>
+      </c>
+      <c r="AX11">
+        <v>0.48</v>
+      </c>
+      <c r="AY11">
+        <v>0.48</v>
+      </c>
+      <c r="AZ11">
+        <v>0.48</v>
+      </c>
+      <c r="BA11">
+        <v>0.48</v>
+      </c>
+      <c r="BB11">
+        <v>0.48</v>
+      </c>
+      <c r="BC11">
+        <v>0.48</v>
+      </c>
+      <c r="BD11">
+        <v>0.48</v>
+      </c>
+      <c r="BE11">
+        <v>0.48</v>
+      </c>
+      <c r="BF11">
+        <v>0.48</v>
+      </c>
+      <c r="BG11">
+        <v>0.48</v>
+      </c>
+      <c r="BH11">
+        <v>0.48</v>
+      </c>
+      <c r="BI11">
+        <v>0.48</v>
+      </c>
+      <c r="BJ11">
+        <v>0.48</v>
+      </c>
+      <c r="BK11">
+        <v>0.48</v>
+      </c>
+      <c r="BL11">
+        <v>0.48</v>
+      </c>
+      <c r="BM11">
+        <v>0.48</v>
+      </c>
+      <c r="BN11">
+        <v>0.48</v>
+      </c>
+      <c r="BO11">
+        <v>0.48</v>
+      </c>
+      <c r="BP11">
+        <v>0.48</v>
+      </c>
+      <c r="BQ11">
+        <v>0.48</v>
+      </c>
+      <c r="BR11">
+        <v>0.48</v>
+      </c>
+      <c r="BS11">
+        <v>0.48</v>
+      </c>
+      <c r="BT11">
+        <v>0.48</v>
+      </c>
+      <c r="BU11">
+        <v>0.48</v>
+      </c>
+      <c r="BV11">
+        <v>0.48</v>
+      </c>
+      <c r="BW11">
+        <v>0.48</v>
+      </c>
+      <c r="BX11">
+        <v>0.48</v>
+      </c>
+      <c r="BY11">
+        <v>0.48</v>
+      </c>
+      <c r="BZ11">
+        <v>0.48</v>
+      </c>
+      <c r="CA11">
+        <v>0.48</v>
+      </c>
+      <c r="CB11">
+        <v>0.48</v>
+      </c>
+      <c r="CC11">
+        <v>0.48</v>
+      </c>
+      <c r="CD11">
+        <v>0.48</v>
+      </c>
+      <c r="CE11">
+        <v>0.48</v>
+      </c>
+      <c r="CF11">
+        <v>0.48</v>
+      </c>
+      <c r="CG11">
+        <v>0.48</v>
+      </c>
+      <c r="CH11">
+        <v>0.48</v>
+      </c>
+      <c r="CI11">
+        <v>0.48</v>
+      </c>
+      <c r="CJ11">
+        <v>0.48</v>
+      </c>
+      <c r="CK11">
+        <v>0.48</v>
+      </c>
+      <c r="CL11">
+        <v>0.48</v>
+      </c>
+      <c r="CM11">
+        <v>0.48</v>
+      </c>
+      <c r="CN11">
+        <v>0.48</v>
+      </c>
+      <c r="CO11">
+        <v>0.48</v>
+      </c>
+      <c r="CP11">
+        <v>0.48</v>
+      </c>
+      <c r="CQ11">
+        <v>0.48</v>
+      </c>
+      <c r="CR11">
+        <v>0.48</v>
+      </c>
+      <c r="CS11">
+        <v>0.48</v>
+      </c>
+      <c r="CT11">
+        <v>0.48</v>
+      </c>
+      <c r="CU11">
+        <v>0.48</v>
+      </c>
+      <c r="CV11">
+        <v>0.48</v>
+      </c>
+      <c r="CW11">
+        <v>0.48</v>
+      </c>
+      <c r="CX11">
+        <v>0.48</v>
+      </c>
+      <c r="CY11">
+        <v>0.48</v>
+      </c>
+      <c r="CZ11">
+        <v>0.48</v>
+      </c>
+      <c r="DA11">
+        <v>0.48</v>
+      </c>
+      <c r="DB11">
+        <v>0.48</v>
+      </c>
+      <c r="DC11">
+        <v>0.48</v>
+      </c>
+      <c r="DD11">
+        <v>0.48</v>
+      </c>
+      <c r="DE11">
+        <v>0.48</v>
+      </c>
+      <c r="DF11">
+        <v>0.48</v>
+      </c>
+      <c r="DG11">
+        <v>0.48</v>
+      </c>
+      <c r="DH11">
+        <v>0.48</v>
+      </c>
+      <c r="DI11">
+        <v>0.48</v>
+      </c>
+      <c r="DJ11">
+        <v>0.48</v>
+      </c>
+      <c r="DK11">
+        <v>0.48</v>
+      </c>
+      <c r="DL11">
+        <v>0.48</v>
+      </c>
+      <c r="DM11">
+        <v>0.48</v>
+      </c>
+      <c r="DN11">
+        <v>0.48</v>
+      </c>
+      <c r="DO11">
+        <v>0.48</v>
+      </c>
+      <c r="DP11">
+        <v>0.48</v>
+      </c>
+      <c r="DQ11">
+        <v>0.48</v>
+      </c>
+      <c r="DR11">
+        <v>0.48</v>
+      </c>
+      <c r="DS11">
+        <v>0.48</v>
+      </c>
+      <c r="DT11">
+        <v>0.48</v>
+      </c>
+      <c r="DU11">
+        <v>0.48</v>
+      </c>
+      <c r="DV11">
+        <v>0.48</v>
+      </c>
+      <c r="DW11">
+        <v>0.48</v>
+      </c>
+      <c r="DX11">
+        <v>0.48</v>
+      </c>
+      <c r="DY11">
+        <v>0.48</v>
+      </c>
+      <c r="DZ11">
+        <v>0.48</v>
+      </c>
+      <c r="EA11">
+        <v>0.48</v>
+      </c>
+      <c r="EB11">
+        <v>0.48</v>
+      </c>
+      <c r="EC11">
+        <v>0.48</v>
+      </c>
+      <c r="ED11">
+        <v>0.48</v>
+      </c>
+      <c r="EE11">
+        <v>0.48</v>
+      </c>
+      <c r="EF11">
+        <v>0.48</v>
+      </c>
+      <c r="EG11">
+        <v>0.48</v>
+      </c>
+      <c r="EH11">
+        <v>0.48</v>
+      </c>
+      <c r="EI11">
+        <v>0.48</v>
+      </c>
+      <c r="EJ11">
+        <v>0.48</v>
+      </c>
+      <c r="EK11">
+        <v>0.48</v>
+      </c>
+      <c r="EL11">
+        <v>0.48</v>
+      </c>
+      <c r="EM11">
+        <v>0.48</v>
+      </c>
+      <c r="EN11">
+        <v>0.48</v>
+      </c>
+      <c r="EO11">
+        <v>0.48</v>
+      </c>
+      <c r="EP11">
+        <v>0.48</v>
+      </c>
+      <c r="EQ11">
+        <v>0.48</v>
+      </c>
+      <c r="ER11">
+        <v>0.48</v>
+      </c>
+      <c r="ES11">
+        <v>0.48</v>
+      </c>
+      <c r="ET11">
+        <v>0.48</v>
+      </c>
+      <c r="EU11">
+        <v>0.48</v>
+      </c>
+      <c r="EV11">
+        <v>0.48</v>
+      </c>
+      <c r="EW11">
+        <v>0.48</v>
+      </c>
+      <c r="EX11">
+        <v>0.48</v>
+      </c>
+      <c r="EY11">
+        <v>0.48</v>
+      </c>
+      <c r="EZ11">
         <v>0.48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lifecycle renovation went through but exported table does not look right.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_BuildingComponent_Input_Labor.xlsx
+++ b/projects/test_building/input/Scenario_BuildingComponent_Input_Labor.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C471B7D7-20F6-454E-B136-D9A94C9DE57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="4305" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="40" yWindow="4300" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -495,7 +496,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -555,165 +556,165 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:EZ11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:EZ11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:EZ11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:EZ11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="156">
-    <tableColumn id="1" name="id_region"/>
-    <tableColumn id="3" name="id_building_component"/>
-    <tableColumn id="4" name="id_building_component_option"/>
-    <tableColumn id="5" name="id_building_action"/>
-    <tableColumn id="6" name="unit"/>
-    <tableColumn id="88" name="1900"/>
-    <tableColumn id="89" name="1901"/>
-    <tableColumn id="90" name="1902"/>
-    <tableColumn id="91" name="1903"/>
-    <tableColumn id="92" name="1904"/>
-    <tableColumn id="93" name="1905"/>
-    <tableColumn id="94" name="1906"/>
-    <tableColumn id="95" name="1907"/>
-    <tableColumn id="96" name="1908"/>
-    <tableColumn id="97" name="1909"/>
-    <tableColumn id="98" name="1910"/>
-    <tableColumn id="99" name="1911"/>
-    <tableColumn id="100" name="1912"/>
-    <tableColumn id="101" name="1913"/>
-    <tableColumn id="102" name="1914"/>
-    <tableColumn id="103" name="1915"/>
-    <tableColumn id="104" name="1916"/>
-    <tableColumn id="105" name="1917"/>
-    <tableColumn id="106" name="1918"/>
-    <tableColumn id="107" name="1919"/>
-    <tableColumn id="108" name="1920"/>
-    <tableColumn id="109" name="1921"/>
-    <tableColumn id="110" name="1922"/>
-    <tableColumn id="111" name="1923"/>
-    <tableColumn id="112" name="1924"/>
-    <tableColumn id="113" name="1925"/>
-    <tableColumn id="114" name="1926"/>
-    <tableColumn id="115" name="1927"/>
-    <tableColumn id="116" name="1928"/>
-    <tableColumn id="117" name="1929"/>
-    <tableColumn id="118" name="1930"/>
-    <tableColumn id="119" name="1931"/>
-    <tableColumn id="120" name="1932"/>
-    <tableColumn id="121" name="1933"/>
-    <tableColumn id="122" name="1934"/>
-    <tableColumn id="123" name="1935"/>
-    <tableColumn id="124" name="1936"/>
-    <tableColumn id="125" name="1937"/>
-    <tableColumn id="126" name="1938"/>
-    <tableColumn id="127" name="1939"/>
-    <tableColumn id="128" name="1940"/>
-    <tableColumn id="129" name="1941"/>
-    <tableColumn id="130" name="1942"/>
-    <tableColumn id="131" name="1943"/>
-    <tableColumn id="132" name="1944"/>
-    <tableColumn id="133" name="1945"/>
-    <tableColumn id="134" name="1946"/>
-    <tableColumn id="135" name="1947"/>
-    <tableColumn id="136" name="1948"/>
-    <tableColumn id="137" name="1949"/>
-    <tableColumn id="138" name="1950"/>
-    <tableColumn id="139" name="1951"/>
-    <tableColumn id="140" name="1952"/>
-    <tableColumn id="141" name="1953"/>
-    <tableColumn id="142" name="1954"/>
-    <tableColumn id="143" name="1955"/>
-    <tableColumn id="144" name="1956"/>
-    <tableColumn id="145" name="1957"/>
-    <tableColumn id="146" name="1958"/>
-    <tableColumn id="147" name="1959"/>
-    <tableColumn id="148" name="1960"/>
-    <tableColumn id="149" name="1961"/>
-    <tableColumn id="150" name="1962"/>
-    <tableColumn id="151" name="1963"/>
-    <tableColumn id="152" name="1964"/>
-    <tableColumn id="153" name="1965"/>
-    <tableColumn id="154" name="1966"/>
-    <tableColumn id="155" name="1967"/>
-    <tableColumn id="156" name="1968"/>
-    <tableColumn id="157" name="1969"/>
-    <tableColumn id="158" name="1970"/>
-    <tableColumn id="159" name="1971"/>
-    <tableColumn id="160" name="1972"/>
-    <tableColumn id="161" name="1973"/>
-    <tableColumn id="162" name="1974"/>
-    <tableColumn id="163" name="1975"/>
-    <tableColumn id="164" name="1976"/>
-    <tableColumn id="165" name="1977"/>
-    <tableColumn id="166" name="1978"/>
-    <tableColumn id="167" name="1979"/>
-    <tableColumn id="168" name="1980"/>
-    <tableColumn id="169" name="1981"/>
-    <tableColumn id="2" name="1982"/>
-    <tableColumn id="48" name="1983"/>
-    <tableColumn id="49" name="1984"/>
-    <tableColumn id="50" name="1985"/>
-    <tableColumn id="51" name="1986"/>
-    <tableColumn id="52" name="1987"/>
-    <tableColumn id="53" name="1988"/>
-    <tableColumn id="54" name="1989"/>
-    <tableColumn id="55" name="1990"/>
-    <tableColumn id="56" name="1991"/>
-    <tableColumn id="57" name="1992"/>
-    <tableColumn id="58" name="1993"/>
-    <tableColumn id="59" name="1994"/>
-    <tableColumn id="60" name="1995"/>
-    <tableColumn id="61" name="1996"/>
-    <tableColumn id="62" name="1997"/>
-    <tableColumn id="63" name="1998"/>
-    <tableColumn id="64" name="1999"/>
-    <tableColumn id="65" name="2000"/>
-    <tableColumn id="66" name="2001"/>
-    <tableColumn id="67" name="2002"/>
-    <tableColumn id="68" name="2003"/>
-    <tableColumn id="69" name="2004"/>
-    <tableColumn id="70" name="2005"/>
-    <tableColumn id="71" name="2006"/>
-    <tableColumn id="72" name="2007"/>
-    <tableColumn id="73" name="2008"/>
-    <tableColumn id="74" name="2009"/>
-    <tableColumn id="7" name="2010"/>
-    <tableColumn id="8" name="2011"/>
-    <tableColumn id="9" name="2012"/>
-    <tableColumn id="10" name="2013"/>
-    <tableColumn id="11" name="2014"/>
-    <tableColumn id="12" name="2015"/>
-    <tableColumn id="13" name="2016"/>
-    <tableColumn id="14" name="2017"/>
-    <tableColumn id="15" name="2018"/>
-    <tableColumn id="16" name="2019"/>
-    <tableColumn id="17" name="2020"/>
-    <tableColumn id="18" name="2021"/>
-    <tableColumn id="19" name="2022"/>
-    <tableColumn id="20" name="2023"/>
-    <tableColumn id="21" name="2024"/>
-    <tableColumn id="22" name="2025"/>
-    <tableColumn id="23" name="2026"/>
-    <tableColumn id="24" name="2027"/>
-    <tableColumn id="25" name="2028"/>
-    <tableColumn id="26" name="2029"/>
-    <tableColumn id="27" name="2030"/>
-    <tableColumn id="28" name="2031"/>
-    <tableColumn id="29" name="2032"/>
-    <tableColumn id="30" name="2033"/>
-    <tableColumn id="31" name="2034"/>
-    <tableColumn id="32" name="2035"/>
-    <tableColumn id="33" name="2036"/>
-    <tableColumn id="34" name="2037"/>
-    <tableColumn id="35" name="2038"/>
-    <tableColumn id="36" name="2039"/>
-    <tableColumn id="37" name="2040"/>
-    <tableColumn id="38" name="2041"/>
-    <tableColumn id="39" name="2042"/>
-    <tableColumn id="40" name="2043"/>
-    <tableColumn id="41" name="2044"/>
-    <tableColumn id="42" name="2045"/>
-    <tableColumn id="43" name="2046"/>
-    <tableColumn id="44" name="2047"/>
-    <tableColumn id="45" name="2048"/>
-    <tableColumn id="46" name="2049"/>
-    <tableColumn id="47" name="2050"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_region"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="id_building_component"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_building_component_option"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="id_building_action"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="unit"/>
+    <tableColumn id="88" xr3:uid="{00000000-0010-0000-0000-000058000000}" name="1900"/>
+    <tableColumn id="89" xr3:uid="{00000000-0010-0000-0000-000059000000}" name="1901"/>
+    <tableColumn id="90" xr3:uid="{00000000-0010-0000-0000-00005A000000}" name="1902"/>
+    <tableColumn id="91" xr3:uid="{00000000-0010-0000-0000-00005B000000}" name="1903"/>
+    <tableColumn id="92" xr3:uid="{00000000-0010-0000-0000-00005C000000}" name="1904"/>
+    <tableColumn id="93" xr3:uid="{00000000-0010-0000-0000-00005D000000}" name="1905"/>
+    <tableColumn id="94" xr3:uid="{00000000-0010-0000-0000-00005E000000}" name="1906"/>
+    <tableColumn id="95" xr3:uid="{00000000-0010-0000-0000-00005F000000}" name="1907"/>
+    <tableColumn id="96" xr3:uid="{00000000-0010-0000-0000-000060000000}" name="1908"/>
+    <tableColumn id="97" xr3:uid="{00000000-0010-0000-0000-000061000000}" name="1909"/>
+    <tableColumn id="98" xr3:uid="{00000000-0010-0000-0000-000062000000}" name="1910"/>
+    <tableColumn id="99" xr3:uid="{00000000-0010-0000-0000-000063000000}" name="1911"/>
+    <tableColumn id="100" xr3:uid="{00000000-0010-0000-0000-000064000000}" name="1912"/>
+    <tableColumn id="101" xr3:uid="{00000000-0010-0000-0000-000065000000}" name="1913"/>
+    <tableColumn id="102" xr3:uid="{00000000-0010-0000-0000-000066000000}" name="1914"/>
+    <tableColumn id="103" xr3:uid="{00000000-0010-0000-0000-000067000000}" name="1915"/>
+    <tableColumn id="104" xr3:uid="{00000000-0010-0000-0000-000068000000}" name="1916"/>
+    <tableColumn id="105" xr3:uid="{00000000-0010-0000-0000-000069000000}" name="1917"/>
+    <tableColumn id="106" xr3:uid="{00000000-0010-0000-0000-00006A000000}" name="1918"/>
+    <tableColumn id="107" xr3:uid="{00000000-0010-0000-0000-00006B000000}" name="1919"/>
+    <tableColumn id="108" xr3:uid="{00000000-0010-0000-0000-00006C000000}" name="1920"/>
+    <tableColumn id="109" xr3:uid="{00000000-0010-0000-0000-00006D000000}" name="1921"/>
+    <tableColumn id="110" xr3:uid="{00000000-0010-0000-0000-00006E000000}" name="1922"/>
+    <tableColumn id="111" xr3:uid="{00000000-0010-0000-0000-00006F000000}" name="1923"/>
+    <tableColumn id="112" xr3:uid="{00000000-0010-0000-0000-000070000000}" name="1924"/>
+    <tableColumn id="113" xr3:uid="{00000000-0010-0000-0000-000071000000}" name="1925"/>
+    <tableColumn id="114" xr3:uid="{00000000-0010-0000-0000-000072000000}" name="1926"/>
+    <tableColumn id="115" xr3:uid="{00000000-0010-0000-0000-000073000000}" name="1927"/>
+    <tableColumn id="116" xr3:uid="{00000000-0010-0000-0000-000074000000}" name="1928"/>
+    <tableColumn id="117" xr3:uid="{00000000-0010-0000-0000-000075000000}" name="1929"/>
+    <tableColumn id="118" xr3:uid="{00000000-0010-0000-0000-000076000000}" name="1930"/>
+    <tableColumn id="119" xr3:uid="{00000000-0010-0000-0000-000077000000}" name="1931"/>
+    <tableColumn id="120" xr3:uid="{00000000-0010-0000-0000-000078000000}" name="1932"/>
+    <tableColumn id="121" xr3:uid="{00000000-0010-0000-0000-000079000000}" name="1933"/>
+    <tableColumn id="122" xr3:uid="{00000000-0010-0000-0000-00007A000000}" name="1934"/>
+    <tableColumn id="123" xr3:uid="{00000000-0010-0000-0000-00007B000000}" name="1935"/>
+    <tableColumn id="124" xr3:uid="{00000000-0010-0000-0000-00007C000000}" name="1936"/>
+    <tableColumn id="125" xr3:uid="{00000000-0010-0000-0000-00007D000000}" name="1937"/>
+    <tableColumn id="126" xr3:uid="{00000000-0010-0000-0000-00007E000000}" name="1938"/>
+    <tableColumn id="127" xr3:uid="{00000000-0010-0000-0000-00007F000000}" name="1939"/>
+    <tableColumn id="128" xr3:uid="{00000000-0010-0000-0000-000080000000}" name="1940"/>
+    <tableColumn id="129" xr3:uid="{00000000-0010-0000-0000-000081000000}" name="1941"/>
+    <tableColumn id="130" xr3:uid="{00000000-0010-0000-0000-000082000000}" name="1942"/>
+    <tableColumn id="131" xr3:uid="{00000000-0010-0000-0000-000083000000}" name="1943"/>
+    <tableColumn id="132" xr3:uid="{00000000-0010-0000-0000-000084000000}" name="1944"/>
+    <tableColumn id="133" xr3:uid="{00000000-0010-0000-0000-000085000000}" name="1945"/>
+    <tableColumn id="134" xr3:uid="{00000000-0010-0000-0000-000086000000}" name="1946"/>
+    <tableColumn id="135" xr3:uid="{00000000-0010-0000-0000-000087000000}" name="1947"/>
+    <tableColumn id="136" xr3:uid="{00000000-0010-0000-0000-000088000000}" name="1948"/>
+    <tableColumn id="137" xr3:uid="{00000000-0010-0000-0000-000089000000}" name="1949"/>
+    <tableColumn id="138" xr3:uid="{00000000-0010-0000-0000-00008A000000}" name="1950"/>
+    <tableColumn id="139" xr3:uid="{00000000-0010-0000-0000-00008B000000}" name="1951"/>
+    <tableColumn id="140" xr3:uid="{00000000-0010-0000-0000-00008C000000}" name="1952"/>
+    <tableColumn id="141" xr3:uid="{00000000-0010-0000-0000-00008D000000}" name="1953"/>
+    <tableColumn id="142" xr3:uid="{00000000-0010-0000-0000-00008E000000}" name="1954"/>
+    <tableColumn id="143" xr3:uid="{00000000-0010-0000-0000-00008F000000}" name="1955"/>
+    <tableColumn id="144" xr3:uid="{00000000-0010-0000-0000-000090000000}" name="1956"/>
+    <tableColumn id="145" xr3:uid="{00000000-0010-0000-0000-000091000000}" name="1957"/>
+    <tableColumn id="146" xr3:uid="{00000000-0010-0000-0000-000092000000}" name="1958"/>
+    <tableColumn id="147" xr3:uid="{00000000-0010-0000-0000-000093000000}" name="1959"/>
+    <tableColumn id="148" xr3:uid="{00000000-0010-0000-0000-000094000000}" name="1960"/>
+    <tableColumn id="149" xr3:uid="{00000000-0010-0000-0000-000095000000}" name="1961"/>
+    <tableColumn id="150" xr3:uid="{00000000-0010-0000-0000-000096000000}" name="1962"/>
+    <tableColumn id="151" xr3:uid="{00000000-0010-0000-0000-000097000000}" name="1963"/>
+    <tableColumn id="152" xr3:uid="{00000000-0010-0000-0000-000098000000}" name="1964"/>
+    <tableColumn id="153" xr3:uid="{00000000-0010-0000-0000-000099000000}" name="1965"/>
+    <tableColumn id="154" xr3:uid="{00000000-0010-0000-0000-00009A000000}" name="1966"/>
+    <tableColumn id="155" xr3:uid="{00000000-0010-0000-0000-00009B000000}" name="1967"/>
+    <tableColumn id="156" xr3:uid="{00000000-0010-0000-0000-00009C000000}" name="1968"/>
+    <tableColumn id="157" xr3:uid="{00000000-0010-0000-0000-00009D000000}" name="1969"/>
+    <tableColumn id="158" xr3:uid="{00000000-0010-0000-0000-00009E000000}" name="1970"/>
+    <tableColumn id="159" xr3:uid="{00000000-0010-0000-0000-00009F000000}" name="1971"/>
+    <tableColumn id="160" xr3:uid="{00000000-0010-0000-0000-0000A0000000}" name="1972"/>
+    <tableColumn id="161" xr3:uid="{00000000-0010-0000-0000-0000A1000000}" name="1973"/>
+    <tableColumn id="162" xr3:uid="{00000000-0010-0000-0000-0000A2000000}" name="1974"/>
+    <tableColumn id="163" xr3:uid="{00000000-0010-0000-0000-0000A3000000}" name="1975"/>
+    <tableColumn id="164" xr3:uid="{00000000-0010-0000-0000-0000A4000000}" name="1976"/>
+    <tableColumn id="165" xr3:uid="{00000000-0010-0000-0000-0000A5000000}" name="1977"/>
+    <tableColumn id="166" xr3:uid="{00000000-0010-0000-0000-0000A6000000}" name="1978"/>
+    <tableColumn id="167" xr3:uid="{00000000-0010-0000-0000-0000A7000000}" name="1979"/>
+    <tableColumn id="168" xr3:uid="{00000000-0010-0000-0000-0000A8000000}" name="1980"/>
+    <tableColumn id="169" xr3:uid="{00000000-0010-0000-0000-0000A9000000}" name="1981"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="1982"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="1983"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="1984"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="1985"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="1986"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="1987"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="1988"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="1989"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="1990"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="1991"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="1992"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="1993"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="1994"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="1995"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="1996"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="1997"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="1998"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="1999"/>
+    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="2000"/>
+    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="2001"/>
+    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="2002"/>
+    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="2003"/>
+    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="2004"/>
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="2005"/>
+    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="2006"/>
+    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="2007"/>
+    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" name="2008"/>
+    <tableColumn id="74" xr3:uid="{00000000-0010-0000-0000-00004A000000}" name="2009"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="2010"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="2011"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2012"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="2013"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2014"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="2015"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="2016"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="2017"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="2018"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="2019"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="2020"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="2021"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="2022"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="2023"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="2024"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="2025"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="2026"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="2027"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="2028"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="2029"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="2030"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="2031"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="2032"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="2033"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="2034"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="2035"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="2036"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="2037"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="2038"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="2039"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="2040"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="2041"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="2042"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="2043"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="2044"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="2045"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="2046"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="2047"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="2048"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="2049"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="2050"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -981,24 +982,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EZ11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="156" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="156" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>9</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>9</v>
       </c>
@@ -2408,7 +2409,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="4" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>9</v>
       </c>
@@ -2878,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9</v>
       </c>
@@ -3348,7 +3349,7 @@
         <v>6.93</v>
       </c>
     </row>
-    <row r="6" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>9</v>
       </c>
@@ -3818,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>9</v>
       </c>
@@ -4288,7 +4289,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="8" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -5228,7 +5229,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="10" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5698,7 +5699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:156" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>

</xml_diff>